<commit_message>
Adiciona cálculo de saldo à planilha
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4275FFFE-ED44-4724-8450-2F7F387BA043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F91A6-F9AB-43F0-B23B-C3A6629CBA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>DESCRIÇÃO</t>
   </si>
@@ -128,6 +128,9 @@
   <si>
     <t>ÁGUA</t>
   </si>
+  <si>
+    <t>SALDO</t>
+  </si>
 </sst>
 </file>
 
@@ -205,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,8 +233,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -439,12 +448,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -547,16 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -568,10 +592,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -583,15 +607,235 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -717,57 +961,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -791,136 +984,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1094,7 +1157,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155.15</c:v>
+                  <c:v>159.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1262,7 +1325,7 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>187.15</c:v>
+                  <c:v>191.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4136</c:v>
@@ -2741,34 +2804,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="B5:J55" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="41">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="7" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="40" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="39">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="38">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="37">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="36">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="35">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="34">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="0" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="33" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2777,35 +2840,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="35" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Moeda">
       <calculatedColumnFormula>RANDBETWEEN(150,956)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="13" totalsRowDxfId="30">
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>RANDBETWEEN(1/8/2025,30/8/2025)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="16" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="7" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3111,7 +3174,7 @@
   <dimension ref="B1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,11 +3205,11 @@
       <c r="C2" s="28">
         <v>8</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
       <c r="L2" s="17" t="s">
         <v>9</v>
       </c>
@@ -3162,71 +3225,71 @@
       <c r="C3" s="28">
         <v>2025</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
       <c r="I3" s="26" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="27">
         <f>H4</f>
-        <v>187.15</v>
+        <v>191.15</v>
       </c>
       <c r="L3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="M3" s="16">
         <f>SUMPRODUCT((R_TABELA[STATUS]=L3)*(MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3)*(R_TABELA[VALOR]))</f>
-        <v>155.15</v>
+        <v>159.15</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="47">
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="44">
         <f>SUM(C6:C55)</f>
-        <v>187.15</v>
+        <v>191.15</v>
       </c>
       <c r="I4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="43">
         <f>SUM(J6:J55)</f>
         <v>4136</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="42" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3269,27 +3332,27 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="str">
+      <c r="B7" s="39" t="str">
         <f t="array" ref="B7">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v>LUZ</v>
       </c>
       <c r="C7" s="19">
         <f t="array" ref="C7">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(2:2))),"")</f>
-        <v>92.15</v>
-      </c>
-      <c r="D7" s="42" t="str">
+        <v>96.15</v>
+      </c>
+      <c r="D7" s="39" t="str">
         <f t="array" ref="D7">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(2:2))),"")</f>
         <v>PENDENTE</v>
       </c>
-      <c r="E7" s="42" t="str">
+      <c r="E7" s="39" t="str">
         <f t="array" ref="E7">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(2:2))),"")</f>
         <v>DESPESA</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="40">
         <f t="array" ref="F7">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v>45891</v>
       </c>
-      <c r="G7" s="42" t="str">
+      <c r="G7" s="39" t="str">
         <f t="array" ref="G7">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v>BOLETO</v>
       </c>
@@ -3297,7 +3360,7 @@
         <f t="array" ref="H7">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(2:2))),"")</f>
         <v>0</v>
       </c>
-      <c r="I7" s="42" t="str">
+      <c r="I7" s="39" t="str">
         <f t="array" ref="I7">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v>RENDIMENTOS</v>
       </c>
@@ -3307,7 +3370,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="str">
+      <c r="B8" s="39" t="str">
         <f t="array" ref="B8">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v>ÁGUA</v>
       </c>
@@ -3315,19 +3378,19 @@
         <f t="array" ref="C8">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(3:3))),"")</f>
         <v>63</v>
       </c>
-      <c r="D8" s="42" t="str">
+      <c r="D8" s="39" t="str">
         <f t="array" ref="D8">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(3:3))),"")</f>
         <v>PENDENTE</v>
       </c>
-      <c r="E8" s="42" t="str">
+      <c r="E8" s="39" t="str">
         <f t="array" ref="E8">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(3:3))),"")</f>
         <v>DESPESA</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="40">
         <f t="array" ref="F8">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v>45891</v>
       </c>
-      <c r="G8" s="42" t="str">
+      <c r="G8" s="39" t="str">
         <f t="array" ref="G8">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v>BOLETO</v>
       </c>
@@ -3335,7 +3398,7 @@
         <f t="array" ref="H8">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(3:3))),"")</f>
         <v>0</v>
       </c>
-      <c r="I8" s="42" t="str">
+      <c r="I8" s="39" t="str">
         <f t="array" ref="I8">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
@@ -3345,7 +3408,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="str">
+      <c r="B9" s="39" t="str">
         <f t="array" ref="B9">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
@@ -3353,19 +3416,19 @@
         <f t="array" ref="C9">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="D9" s="42" t="str">
+      <c r="D9" s="39" t="str">
         <f t="array" ref="D9">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="E9" s="42" t="str">
+      <c r="E9" s="39" t="str">
         <f t="array" ref="E9">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="F9" s="43" t="str">
+      <c r="F9" s="40" t="str">
         <f t="array" ref="F9">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="G9" s="42" t="str">
+      <c r="G9" s="39" t="str">
         <f t="array" ref="G9">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
@@ -3373,7 +3436,7 @@
         <f t="array" ref="H9">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="I9" s="42" t="str">
+      <c r="I9" s="39" t="str">
         <f t="array" ref="I9">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
@@ -3383,7 +3446,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="42" t="str">
+      <c r="B10" s="39" t="str">
         <f t="array" ref="B10">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
@@ -3391,19 +3454,19 @@
         <f t="array" ref="C10">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="D10" s="42" t="str">
+      <c r="D10" s="39" t="str">
         <f t="array" ref="D10">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="E10" s="42" t="str">
+      <c r="E10" s="39" t="str">
         <f t="array" ref="E10">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="F10" s="43" t="str">
+      <c r="F10" s="40" t="str">
         <f t="array" ref="F10">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="G10" s="42" t="str">
+      <c r="G10" s="39" t="str">
         <f t="array" ref="G10">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
@@ -3411,7 +3474,7 @@
         <f t="array" ref="H10">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="I10" s="42" t="str">
+      <c r="I10" s="39" t="str">
         <f t="array" ref="I10">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
@@ -3421,7 +3484,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="str">
+      <c r="B11" s="39" t="str">
         <f t="array" ref="B11">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
@@ -3429,19 +3492,19 @@
         <f t="array" ref="C11">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="D11" s="42" t="str">
+      <c r="D11" s="39" t="str">
         <f t="array" ref="D11">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="E11" s="42" t="str">
+      <c r="E11" s="39" t="str">
         <f t="array" ref="E11">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="F11" s="43" t="str">
+      <c r="F11" s="40" t="str">
         <f t="array" ref="F11">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="G11" s="42" t="str">
+      <c r="G11" s="39" t="str">
         <f t="array" ref="G11">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
@@ -3449,7 +3512,7 @@
         <f t="array" ref="H11">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="I11" s="42" t="str">
+      <c r="I11" s="39" t="str">
         <f t="array" ref="I11">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
@@ -3459,7 +3522,7 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="str">
+      <c r="B12" s="39" t="str">
         <f t="array" ref="B12">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
@@ -3467,19 +3530,19 @@
         <f t="array" ref="C12">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="D12" s="42" t="str">
+      <c r="D12" s="39" t="str">
         <f t="array" ref="D12">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="E12" s="42" t="str">
+      <c r="E12" s="39" t="str">
         <f t="array" ref="E12">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="F12" s="43" t="str">
+      <c r="F12" s="40" t="str">
         <f t="array" ref="F12">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="G12" s="42" t="str">
+      <c r="G12" s="39" t="str">
         <f t="array" ref="G12">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
@@ -3487,7 +3550,7 @@
         <f t="array" ref="H12">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="I12" s="42" t="str">
+      <c r="I12" s="39" t="str">
         <f t="array" ref="I12">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
@@ -3497,7 +3560,7 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="str">
+      <c r="B13" s="39" t="str">
         <f t="array" ref="B13">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
@@ -3505,19 +3568,19 @@
         <f t="array" ref="C13">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="D13" s="42" t="str">
+      <c r="D13" s="39" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="E13" s="42" t="str">
+      <c r="E13" s="39" t="str">
         <f t="array" ref="E13">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="F13" s="43" t="str">
+      <c r="F13" s="40" t="str">
         <f t="array" ref="F13">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="G13" s="42" t="str">
+      <c r="G13" s="39" t="str">
         <f t="array" ref="G13">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
@@ -3525,7 +3588,7 @@
         <f t="array" ref="H13">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="I13" s="42" t="str">
+      <c r="I13" s="39" t="str">
         <f t="array" ref="I13">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
@@ -3535,7 +3598,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="42" t="str">
+      <c r="B14" s="39" t="str">
         <f t="array" ref="B14">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
@@ -3543,19 +3606,19 @@
         <f t="array" ref="C14">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="D14" s="42" t="str">
+      <c r="D14" s="39" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="E14" s="42" t="str">
+      <c r="E14" s="39" t="str">
         <f t="array" ref="E14">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="F14" s="43" t="str">
+      <c r="F14" s="40" t="str">
         <f t="array" ref="F14">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="G14" s="42" t="str">
+      <c r="G14" s="39" t="str">
         <f t="array" ref="G14">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
@@ -3563,7 +3626,7 @@
         <f t="array" ref="H14">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="I14" s="42" t="str">
+      <c r="I14" s="39" t="str">
         <f t="array" ref="I14">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
@@ -3572,8 +3635,8 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="42" t="str">
+    <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="39" t="str">
         <f t="array" ref="B15">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
@@ -3581,19 +3644,19 @@
         <f t="array" ref="C15">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="D15" s="42" t="str">
+      <c r="D15" s="39" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="E15" s="42" t="str">
+      <c r="E15" s="39" t="str">
         <f t="array" ref="E15">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="F15" s="43" t="str">
+      <c r="F15" s="40" t="str">
         <f t="array" ref="F15">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="G15" s="42" t="str">
+      <c r="G15" s="39" t="str">
         <f t="array" ref="G15">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
@@ -3601,7 +3664,7 @@
         <f t="array" ref="H15">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="I15" s="42" t="str">
+      <c r="I15" s="39" t="str">
         <f t="array" ref="I15">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
@@ -3611,7 +3674,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="str">
+      <c r="B16" s="39" t="str">
         <f t="array" ref="B16">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
@@ -3619,19 +3682,19 @@
         <f t="array" ref="C16">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="D16" s="42" t="str">
+      <c r="D16" s="39" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="E16" s="42" t="str">
+      <c r="E16" s="39" t="str">
         <f t="array" ref="E16">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="F16" s="43" t="str">
+      <c r="F16" s="40" t="str">
         <f t="array" ref="F16">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="G16" s="42" t="str">
+      <c r="G16" s="39" t="str">
         <f t="array" ref="G16">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
@@ -3639,7 +3702,7 @@
         <f t="array" ref="H16">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="I16" s="42" t="str">
+      <c r="I16" s="39" t="str">
         <f t="array" ref="I16">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
@@ -3647,9 +3710,16 @@
         <f t="array" ref="J16">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="str">
+      <c r="L16" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="47">
+        <f>J4-H4</f>
+        <v>3944.85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="39" t="str">
         <f t="array" ref="B17">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
@@ -3657,19 +3727,19 @@
         <f t="array" ref="C17">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="D17" s="42" t="str">
+      <c r="D17" s="39" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="E17" s="42" t="str">
+      <c r="E17" s="39" t="str">
         <f t="array" ref="E17">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="F17" s="43" t="str">
+      <c r="F17" s="40" t="str">
         <f t="array" ref="F17">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="G17" s="42" t="str">
+      <c r="G17" s="39" t="str">
         <f t="array" ref="G17">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
@@ -3677,7 +3747,7 @@
         <f t="array" ref="H17">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="I17" s="42" t="str">
+      <c r="I17" s="39" t="str">
         <f t="array" ref="I17">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
@@ -3685,9 +3755,11 @@
         <f t="array" ref="J17">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="str">
+      <c r="L17" s="50"/>
+      <c r="M17" s="48"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="39" t="str">
         <f t="array" ref="B18">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
@@ -3695,19 +3767,19 @@
         <f t="array" ref="C18">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="D18" s="42" t="str">
+      <c r="D18" s="39" t="str">
         <f t="array" ref="D18">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="E18" s="42" t="str">
+      <c r="E18" s="39" t="str">
         <f t="array" ref="E18">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="F18" s="43" t="str">
+      <c r="F18" s="40" t="str">
         <f t="array" ref="F18">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="G18" s="42" t="str">
+      <c r="G18" s="39" t="str">
         <f t="array" ref="G18">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
@@ -3715,7 +3787,7 @@
         <f t="array" ref="H18">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="I18" s="42" t="str">
+      <c r="I18" s="39" t="str">
         <f t="array" ref="I18">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
@@ -3724,8 +3796,8 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="str">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="39" t="str">
         <f t="array" ref="B19">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
@@ -3733,19 +3805,19 @@
         <f t="array" ref="C19">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="D19" s="42" t="str">
+      <c r="D19" s="39" t="str">
         <f t="array" ref="D19">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="E19" s="42" t="str">
+      <c r="E19" s="39" t="str">
         <f t="array" ref="E19">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="F19" s="43" t="str">
+      <c r="F19" s="40" t="str">
         <f t="array" ref="F19">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="G19" s="42" t="str">
+      <c r="G19" s="39" t="str">
         <f t="array" ref="G19">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
@@ -3753,7 +3825,7 @@
         <f t="array" ref="H19">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="I19" s="42" t="str">
+      <c r="I19" s="39" t="str">
         <f t="array" ref="I19">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
@@ -3762,8 +3834,8 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="str">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="39" t="str">
         <f t="array" ref="B20">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
@@ -3771,19 +3843,19 @@
         <f t="array" ref="C20">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="D20" s="42" t="str">
+      <c r="D20" s="39" t="str">
         <f t="array" ref="D20">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="E20" s="42" t="str">
+      <c r="E20" s="39" t="str">
         <f t="array" ref="E20">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="F20" s="43" t="str">
+      <c r="F20" s="40" t="str">
         <f t="array" ref="F20">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="G20" s="42" t="str">
+      <c r="G20" s="39" t="str">
         <f t="array" ref="G20">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
@@ -3791,7 +3863,7 @@
         <f t="array" ref="H20">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="I20" s="42" t="str">
+      <c r="I20" s="39" t="str">
         <f t="array" ref="I20">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
@@ -3800,8 +3872,8 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="42" t="str">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="39" t="str">
         <f t="array" ref="B21">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
@@ -3809,19 +3881,19 @@
         <f t="array" ref="C21">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="D21" s="42" t="str">
+      <c r="D21" s="39" t="str">
         <f t="array" ref="D21">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="E21" s="42" t="str">
+      <c r="E21" s="39" t="str">
         <f t="array" ref="E21">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="F21" s="43" t="str">
+      <c r="F21" s="40" t="str">
         <f t="array" ref="F21">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="G21" s="42" t="str">
+      <c r="G21" s="39" t="str">
         <f t="array" ref="G21">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
@@ -3829,7 +3901,7 @@
         <f t="array" ref="H21">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="I21" s="42" t="str">
+      <c r="I21" s="39" t="str">
         <f t="array" ref="I21">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
@@ -3838,8 +3910,8 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="42" t="str">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="39" t="str">
         <f t="array" ref="B22">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
@@ -3847,19 +3919,19 @@
         <f t="array" ref="C22">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="D22" s="42" t="str">
+      <c r="D22" s="39" t="str">
         <f t="array" ref="D22">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="E22" s="42" t="str">
+      <c r="E22" s="39" t="str">
         <f t="array" ref="E22">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="F22" s="43" t="str">
+      <c r="F22" s="40" t="str">
         <f t="array" ref="F22">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="G22" s="42" t="str">
+      <c r="G22" s="39" t="str">
         <f t="array" ref="G22">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
@@ -3867,7 +3939,7 @@
         <f t="array" ref="H22">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="I22" s="42" t="str">
+      <c r="I22" s="39" t="str">
         <f t="array" ref="I22">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
@@ -3876,8 +3948,8 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="str">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="39" t="str">
         <f t="array" ref="B23">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
@@ -3885,19 +3957,19 @@
         <f t="array" ref="C23">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="D23" s="42" t="str">
+      <c r="D23" s="39" t="str">
         <f t="array" ref="D23">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="E23" s="42" t="str">
+      <c r="E23" s="39" t="str">
         <f t="array" ref="E23">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="F23" s="43" t="str">
+      <c r="F23" s="40" t="str">
         <f t="array" ref="F23">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="G23" s="42" t="str">
+      <c r="G23" s="39" t="str">
         <f t="array" ref="G23">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
@@ -3905,7 +3977,7 @@
         <f t="array" ref="H23">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="I23" s="42" t="str">
+      <c r="I23" s="39" t="str">
         <f t="array" ref="I23">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
@@ -3914,8 +3986,8 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="str">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="39" t="str">
         <f t="array" ref="B24">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
@@ -3923,19 +3995,19 @@
         <f t="array" ref="C24">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="D24" s="42" t="str">
+      <c r="D24" s="39" t="str">
         <f t="array" ref="D24">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="E24" s="42" t="str">
+      <c r="E24" s="39" t="str">
         <f t="array" ref="E24">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="F24" s="43" t="str">
+      <c r="F24" s="40" t="str">
         <f t="array" ref="F24">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="G24" s="42" t="str">
+      <c r="G24" s="39" t="str">
         <f t="array" ref="G24">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
@@ -3943,7 +4015,7 @@
         <f t="array" ref="H24">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="I24" s="42" t="str">
+      <c r="I24" s="39" t="str">
         <f t="array" ref="I24">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
@@ -3952,8 +4024,8 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="str">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="39" t="str">
         <f t="array" ref="B25">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
@@ -3961,19 +4033,19 @@
         <f t="array" ref="C25">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="D25" s="42" t="str">
+      <c r="D25" s="39" t="str">
         <f t="array" ref="D25">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="E25" s="42" t="str">
+      <c r="E25" s="39" t="str">
         <f t="array" ref="E25">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="F25" s="43" t="str">
+      <c r="F25" s="40" t="str">
         <f t="array" ref="F25">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="G25" s="42" t="str">
+      <c r="G25" s="39" t="str">
         <f t="array" ref="G25">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
@@ -3981,7 +4053,7 @@
         <f t="array" ref="H25">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="I25" s="42" t="str">
+      <c r="I25" s="39" t="str">
         <f t="array" ref="I25">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
@@ -3990,8 +4062,8 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="str">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="39" t="str">
         <f t="array" ref="B26">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
@@ -3999,19 +4071,19 @@
         <f t="array" ref="C26">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="D26" s="42" t="str">
+      <c r="D26" s="39" t="str">
         <f t="array" ref="D26">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="E26" s="42" t="str">
+      <c r="E26" s="39" t="str">
         <f t="array" ref="E26">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="F26" s="43" t="str">
+      <c r="F26" s="40" t="str">
         <f t="array" ref="F26">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="G26" s="42" t="str">
+      <c r="G26" s="39" t="str">
         <f t="array" ref="G26">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
@@ -4019,7 +4091,7 @@
         <f t="array" ref="H26">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="I26" s="42" t="str">
+      <c r="I26" s="39" t="str">
         <f t="array" ref="I26">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
@@ -4028,8 +4100,8 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="str">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="39" t="str">
         <f t="array" ref="B27">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
@@ -4037,19 +4109,19 @@
         <f t="array" ref="C27">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="D27" s="42" t="str">
+      <c r="D27" s="39" t="str">
         <f t="array" ref="D27">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="E27" s="42" t="str">
+      <c r="E27" s="39" t="str">
         <f t="array" ref="E27">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="F27" s="43" t="str">
+      <c r="F27" s="40" t="str">
         <f t="array" ref="F27">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="G27" s="42" t="str">
+      <c r="G27" s="39" t="str">
         <f t="array" ref="G27">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
@@ -4057,7 +4129,7 @@
         <f t="array" ref="H27">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="I27" s="42" t="str">
+      <c r="I27" s="39" t="str">
         <f t="array" ref="I27">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
@@ -4066,8 +4138,8 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="str">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="39" t="str">
         <f t="array" ref="B28">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
@@ -4075,19 +4147,19 @@
         <f t="array" ref="C28">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="D28" s="42" t="str">
+      <c r="D28" s="39" t="str">
         <f t="array" ref="D28">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="E28" s="42" t="str">
+      <c r="E28" s="39" t="str">
         <f t="array" ref="E28">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="F28" s="43" t="str">
+      <c r="F28" s="40" t="str">
         <f t="array" ref="F28">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="G28" s="42" t="str">
+      <c r="G28" s="39" t="str">
         <f t="array" ref="G28">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
@@ -4095,7 +4167,7 @@
         <f t="array" ref="H28">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="I28" s="42" t="str">
+      <c r="I28" s="39" t="str">
         <f t="array" ref="I28">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
@@ -4104,8 +4176,8 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="str">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="39" t="str">
         <f t="array" ref="B29">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
@@ -4113,19 +4185,19 @@
         <f t="array" ref="C29">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="D29" s="42" t="str">
+      <c r="D29" s="39" t="str">
         <f t="array" ref="D29">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="E29" s="42" t="str">
+      <c r="E29" s="39" t="str">
         <f t="array" ref="E29">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="F29" s="43" t="str">
+      <c r="F29" s="40" t="str">
         <f t="array" ref="F29">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="G29" s="42" t="str">
+      <c r="G29" s="39" t="str">
         <f t="array" ref="G29">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
@@ -4133,7 +4205,7 @@
         <f t="array" ref="H29">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="I29" s="42" t="str">
+      <c r="I29" s="39" t="str">
         <f t="array" ref="I29">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
@@ -4142,8 +4214,8 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="str">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="39" t="str">
         <f t="array" ref="B30">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
@@ -4151,19 +4223,19 @@
         <f t="array" ref="C30">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="D30" s="42" t="str">
+      <c r="D30" s="39" t="str">
         <f t="array" ref="D30">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="E30" s="42" t="str">
+      <c r="E30" s="39" t="str">
         <f t="array" ref="E30">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="F30" s="43" t="str">
+      <c r="F30" s="40" t="str">
         <f t="array" ref="F30">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="G30" s="42" t="str">
+      <c r="G30" s="39" t="str">
         <f t="array" ref="G30">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
@@ -4171,7 +4243,7 @@
         <f t="array" ref="H30">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="I30" s="42" t="str">
+      <c r="I30" s="39" t="str">
         <f t="array" ref="I30">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
@@ -4180,8 +4252,8 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="42" t="str">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="39" t="str">
         <f t="array" ref="B31">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
@@ -4189,19 +4261,19 @@
         <f t="array" ref="C31">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="D31" s="42" t="str">
+      <c r="D31" s="39" t="str">
         <f t="array" ref="D31">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="E31" s="42" t="str">
+      <c r="E31" s="39" t="str">
         <f t="array" ref="E31">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="F31" s="43" t="str">
+      <c r="F31" s="40" t="str">
         <f t="array" ref="F31">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="G31" s="42" t="str">
+      <c r="G31" s="39" t="str">
         <f t="array" ref="G31">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
@@ -4209,7 +4281,7 @@
         <f t="array" ref="H31">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="I31" s="42" t="str">
+      <c r="I31" s="39" t="str">
         <f t="array" ref="I31">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
@@ -4218,8 +4290,8 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="str">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="39" t="str">
         <f t="array" ref="B32">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
@@ -4227,19 +4299,19 @@
         <f t="array" ref="C32">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="D32" s="42" t="str">
+      <c r="D32" s="39" t="str">
         <f t="array" ref="D32">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="E32" s="42" t="str">
+      <c r="E32" s="39" t="str">
         <f t="array" ref="E32">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="F32" s="43" t="str">
+      <c r="F32" s="40" t="str">
         <f t="array" ref="F32">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="G32" s="42" t="str">
+      <c r="G32" s="39" t="str">
         <f t="array" ref="G32">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
@@ -4247,7 +4319,7 @@
         <f t="array" ref="H32">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="I32" s="42" t="str">
+      <c r="I32" s="39" t="str">
         <f t="array" ref="I32">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
@@ -4257,7 +4329,7 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="42" t="str">
+      <c r="B33" s="39" t="str">
         <f t="array" ref="B33">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
@@ -4265,19 +4337,19 @@
         <f t="array" ref="C33">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="D33" s="42" t="str">
+      <c r="D33" s="39" t="str">
         <f t="array" ref="D33">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="E33" s="42" t="str">
+      <c r="E33" s="39" t="str">
         <f t="array" ref="E33">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="F33" s="43" t="str">
+      <c r="F33" s="40" t="str">
         <f t="array" ref="F33">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="G33" s="42" t="str">
+      <c r="G33" s="39" t="str">
         <f t="array" ref="G33">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
@@ -4285,7 +4357,7 @@
         <f t="array" ref="H33">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="I33" s="42" t="str">
+      <c r="I33" s="39" t="str">
         <f t="array" ref="I33">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
@@ -4295,7 +4367,7 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="42" t="str">
+      <c r="B34" s="39" t="str">
         <f t="array" ref="B34">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
@@ -4303,19 +4375,19 @@
         <f t="array" ref="C34">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="D34" s="42" t="str">
+      <c r="D34" s="39" t="str">
         <f t="array" ref="D34">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="E34" s="42" t="str">
+      <c r="E34" s="39" t="str">
         <f t="array" ref="E34">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="F34" s="43" t="str">
+      <c r="F34" s="40" t="str">
         <f t="array" ref="F34">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="G34" s="42" t="str">
+      <c r="G34" s="39" t="str">
         <f t="array" ref="G34">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
@@ -4323,7 +4395,7 @@
         <f t="array" ref="H34">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="I34" s="42" t="str">
+      <c r="I34" s="39" t="str">
         <f t="array" ref="I34">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
@@ -4333,7 +4405,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="42" t="str">
+      <c r="B35" s="39" t="str">
         <f t="array" ref="B35">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
@@ -4341,19 +4413,19 @@
         <f t="array" ref="C35">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="D35" s="42" t="str">
+      <c r="D35" s="39" t="str">
         <f t="array" ref="D35">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="E35" s="42" t="str">
+      <c r="E35" s="39" t="str">
         <f t="array" ref="E35">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="F35" s="43" t="str">
+      <c r="F35" s="40" t="str">
         <f t="array" ref="F35">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="G35" s="42" t="str">
+      <c r="G35" s="39" t="str">
         <f t="array" ref="G35">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
@@ -4361,7 +4433,7 @@
         <f t="array" ref="H35">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="I35" s="42" t="str">
+      <c r="I35" s="39" t="str">
         <f t="array" ref="I35">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
@@ -4371,7 +4443,7 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="42" t="str">
+      <c r="B36" s="39" t="str">
         <f t="array" ref="B36">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
@@ -4379,19 +4451,19 @@
         <f t="array" ref="C36">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="D36" s="42" t="str">
+      <c r="D36" s="39" t="str">
         <f t="array" ref="D36">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="E36" s="42" t="str">
+      <c r="E36" s="39" t="str">
         <f t="array" ref="E36">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="F36" s="43" t="str">
+      <c r="F36" s="40" t="str">
         <f t="array" ref="F36">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="G36" s="42" t="str">
+      <c r="G36" s="39" t="str">
         <f t="array" ref="G36">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
@@ -4399,7 +4471,7 @@
         <f t="array" ref="H36">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="I36" s="42" t="str">
+      <c r="I36" s="39" t="str">
         <f t="array" ref="I36">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
@@ -4409,7 +4481,7 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="42" t="str">
+      <c r="B37" s="39" t="str">
         <f t="array" ref="B37">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
@@ -4417,19 +4489,19 @@
         <f t="array" ref="C37">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="D37" s="42" t="str">
+      <c r="D37" s="39" t="str">
         <f t="array" ref="D37">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="E37" s="42" t="str">
+      <c r="E37" s="39" t="str">
         <f t="array" ref="E37">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="F37" s="43" t="str">
+      <c r="F37" s="40" t="str">
         <f t="array" ref="F37">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="G37" s="42" t="str">
+      <c r="G37" s="39" t="str">
         <f t="array" ref="G37">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
@@ -4437,7 +4509,7 @@
         <f t="array" ref="H37">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="I37" s="42" t="str">
+      <c r="I37" s="39" t="str">
         <f t="array" ref="I37">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
@@ -4447,7 +4519,7 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="42" t="str">
+      <c r="B38" s="39" t="str">
         <f t="array" ref="B38">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
@@ -4455,19 +4527,19 @@
         <f t="array" ref="C38">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="D38" s="42" t="str">
+      <c r="D38" s="39" t="str">
         <f t="array" ref="D38">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="E38" s="42" t="str">
+      <c r="E38" s="39" t="str">
         <f t="array" ref="E38">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="F38" s="43" t="str">
+      <c r="F38" s="40" t="str">
         <f t="array" ref="F38">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="G38" s="42" t="str">
+      <c r="G38" s="39" t="str">
         <f t="array" ref="G38">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
@@ -4475,7 +4547,7 @@
         <f t="array" ref="H38">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="I38" s="42" t="str">
+      <c r="I38" s="39" t="str">
         <f t="array" ref="I38">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
@@ -4485,7 +4557,7 @@
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="42" t="str">
+      <c r="B39" s="39" t="str">
         <f t="array" ref="B39">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
@@ -4493,19 +4565,19 @@
         <f t="array" ref="C39">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="D39" s="42" t="str">
+      <c r="D39" s="39" t="str">
         <f t="array" ref="D39">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="E39" s="42" t="str">
+      <c r="E39" s="39" t="str">
         <f t="array" ref="E39">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="F39" s="43" t="str">
+      <c r="F39" s="40" t="str">
         <f t="array" ref="F39">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="G39" s="42" t="str">
+      <c r="G39" s="39" t="str">
         <f t="array" ref="G39">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
@@ -4513,7 +4585,7 @@
         <f t="array" ref="H39">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="I39" s="42" t="str">
+      <c r="I39" s="39" t="str">
         <f t="array" ref="I39">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
@@ -4523,7 +4595,7 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="42" t="str">
+      <c r="B40" s="39" t="str">
         <f t="array" ref="B40">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
@@ -4531,19 +4603,19 @@
         <f t="array" ref="C40">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="D40" s="42" t="str">
+      <c r="D40" s="39" t="str">
         <f t="array" ref="D40">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="E40" s="42" t="str">
+      <c r="E40" s="39" t="str">
         <f t="array" ref="E40">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="F40" s="43" t="str">
+      <c r="F40" s="40" t="str">
         <f t="array" ref="F40">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="G40" s="42" t="str">
+      <c r="G40" s="39" t="str">
         <f t="array" ref="G40">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
@@ -4551,7 +4623,7 @@
         <f t="array" ref="H40">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="I40" s="42" t="str">
+      <c r="I40" s="39" t="str">
         <f t="array" ref="I40">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
@@ -4561,7 +4633,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="42" t="str">
+      <c r="B41" s="39" t="str">
         <f t="array" ref="B41">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
@@ -4569,19 +4641,19 @@
         <f t="array" ref="C41">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="D41" s="42" t="str">
+      <c r="D41" s="39" t="str">
         <f t="array" ref="D41">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="E41" s="42" t="str">
+      <c r="E41" s="39" t="str">
         <f t="array" ref="E41">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="F41" s="43" t="str">
+      <c r="F41" s="40" t="str">
         <f t="array" ref="F41">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="G41" s="42" t="str">
+      <c r="G41" s="39" t="str">
         <f t="array" ref="G41">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
@@ -4589,7 +4661,7 @@
         <f t="array" ref="H41">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="I41" s="42" t="str">
+      <c r="I41" s="39" t="str">
         <f t="array" ref="I41">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
@@ -4599,7 +4671,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="42" t="str">
+      <c r="B42" s="39" t="str">
         <f t="array" ref="B42">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
@@ -4607,19 +4679,19 @@
         <f t="array" ref="C42">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="D42" s="42" t="str">
+      <c r="D42" s="39" t="str">
         <f t="array" ref="D42">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="E42" s="42" t="str">
+      <c r="E42" s="39" t="str">
         <f t="array" ref="E42">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="F42" s="43" t="str">
+      <c r="F42" s="40" t="str">
         <f t="array" ref="F42">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="G42" s="42" t="str">
+      <c r="G42" s="39" t="str">
         <f t="array" ref="G42">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
@@ -4627,7 +4699,7 @@
         <f t="array" ref="H42">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="I42" s="42" t="str">
+      <c r="I42" s="39" t="str">
         <f t="array" ref="I42">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
@@ -4637,7 +4709,7 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="42" t="str">
+      <c r="B43" s="39" t="str">
         <f t="array" ref="B43">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
@@ -4645,19 +4717,19 @@
         <f t="array" ref="C43">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="D43" s="42" t="str">
+      <c r="D43" s="39" t="str">
         <f t="array" ref="D43">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="E43" s="42" t="str">
+      <c r="E43" s="39" t="str">
         <f t="array" ref="E43">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="F43" s="43" t="str">
+      <c r="F43" s="40" t="str">
         <f t="array" ref="F43">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="G43" s="42" t="str">
+      <c r="G43" s="39" t="str">
         <f t="array" ref="G43">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
@@ -4665,7 +4737,7 @@
         <f t="array" ref="H43">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="I43" s="42" t="str">
+      <c r="I43" s="39" t="str">
         <f t="array" ref="I43">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
@@ -4675,7 +4747,7 @@
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="42" t="str">
+      <c r="B44" s="39" t="str">
         <f t="array" ref="B44">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
@@ -4683,19 +4755,19 @@
         <f t="array" ref="C44">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="D44" s="42" t="str">
+      <c r="D44" s="39" t="str">
         <f t="array" ref="D44">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="E44" s="42" t="str">
+      <c r="E44" s="39" t="str">
         <f t="array" ref="E44">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="F44" s="43" t="str">
+      <c r="F44" s="40" t="str">
         <f t="array" ref="F44">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="G44" s="42" t="str">
+      <c r="G44" s="39" t="str">
         <f t="array" ref="G44">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
@@ -4703,7 +4775,7 @@
         <f t="array" ref="H44">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="I44" s="42" t="str">
+      <c r="I44" s="39" t="str">
         <f t="array" ref="I44">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
@@ -4713,7 +4785,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="42" t="str">
+      <c r="B45" s="39" t="str">
         <f t="array" ref="B45">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
@@ -4721,19 +4793,19 @@
         <f t="array" ref="C45">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="D45" s="42" t="str">
+      <c r="D45" s="39" t="str">
         <f t="array" ref="D45">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="E45" s="42" t="str">
+      <c r="E45" s="39" t="str">
         <f t="array" ref="E45">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="F45" s="43" t="str">
+      <c r="F45" s="40" t="str">
         <f t="array" ref="F45">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="G45" s="42" t="str">
+      <c r="G45" s="39" t="str">
         <f t="array" ref="G45">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
@@ -4741,7 +4813,7 @@
         <f t="array" ref="H45">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="I45" s="42" t="str">
+      <c r="I45" s="39" t="str">
         <f t="array" ref="I45">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
@@ -4751,7 +4823,7 @@
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="42" t="str">
+      <c r="B46" s="39" t="str">
         <f t="array" ref="B46">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
@@ -4759,19 +4831,19 @@
         <f t="array" ref="C46">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="D46" s="42" t="str">
+      <c r="D46" s="39" t="str">
         <f t="array" ref="D46">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="E46" s="42" t="str">
+      <c r="E46" s="39" t="str">
         <f t="array" ref="E46">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="F46" s="43" t="str">
+      <c r="F46" s="40" t="str">
         <f t="array" ref="F46">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="G46" s="42" t="str">
+      <c r="G46" s="39" t="str">
         <f t="array" ref="G46">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
@@ -4779,7 +4851,7 @@
         <f t="array" ref="H46">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="I46" s="42" t="str">
+      <c r="I46" s="39" t="str">
         <f t="array" ref="I46">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
@@ -4789,7 +4861,7 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="42" t="str">
+      <c r="B47" s="39" t="str">
         <f t="array" ref="B47">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
@@ -4797,19 +4869,19 @@
         <f t="array" ref="C47">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="D47" s="42" t="str">
+      <c r="D47" s="39" t="str">
         <f t="array" ref="D47">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="E47" s="42" t="str">
+      <c r="E47" s="39" t="str">
         <f t="array" ref="E47">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="F47" s="43" t="str">
+      <c r="F47" s="40" t="str">
         <f t="array" ref="F47">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="G47" s="42" t="str">
+      <c r="G47" s="39" t="str">
         <f t="array" ref="G47">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
@@ -4817,7 +4889,7 @@
         <f t="array" ref="H47">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="I47" s="42" t="str">
+      <c r="I47" s="39" t="str">
         <f t="array" ref="I47">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
@@ -4827,7 +4899,7 @@
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="42" t="str">
+      <c r="B48" s="39" t="str">
         <f t="array" ref="B48">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
@@ -4835,19 +4907,19 @@
         <f t="array" ref="C48">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="D48" s="42" t="str">
+      <c r="D48" s="39" t="str">
         <f t="array" ref="D48">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="E48" s="42" t="str">
+      <c r="E48" s="39" t="str">
         <f t="array" ref="E48">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="F48" s="43" t="str">
+      <c r="F48" s="40" t="str">
         <f t="array" ref="F48">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="G48" s="42" t="str">
+      <c r="G48" s="39" t="str">
         <f t="array" ref="G48">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
@@ -4855,7 +4927,7 @@
         <f t="array" ref="H48">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="I48" s="42" t="str">
+      <c r="I48" s="39" t="str">
         <f t="array" ref="I48">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
@@ -4865,7 +4937,7 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="42" t="str">
+      <c r="B49" s="39" t="str">
         <f t="array" ref="B49">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
@@ -4873,19 +4945,19 @@
         <f t="array" ref="C49">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="D49" s="42" t="str">
+      <c r="D49" s="39" t="str">
         <f t="array" ref="D49">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="E49" s="42" t="str">
+      <c r="E49" s="39" t="str">
         <f t="array" ref="E49">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="F49" s="43" t="str">
+      <c r="F49" s="40" t="str">
         <f t="array" ref="F49">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="G49" s="42" t="str">
+      <c r="G49" s="39" t="str">
         <f t="array" ref="G49">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
@@ -4893,7 +4965,7 @@
         <f t="array" ref="H49">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="I49" s="42" t="str">
+      <c r="I49" s="39" t="str">
         <f t="array" ref="I49">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
@@ -4903,7 +4975,7 @@
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="42" t="str">
+      <c r="B50" s="39" t="str">
         <f t="array" ref="B50">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
@@ -4911,19 +4983,19 @@
         <f t="array" ref="C50">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="D50" s="42" t="str">
+      <c r="D50" s="39" t="str">
         <f t="array" ref="D50">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="E50" s="42" t="str">
+      <c r="E50" s="39" t="str">
         <f t="array" ref="E50">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="F50" s="43" t="str">
+      <c r="F50" s="40" t="str">
         <f t="array" ref="F50">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="G50" s="42" t="str">
+      <c r="G50" s="39" t="str">
         <f t="array" ref="G50">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
@@ -4931,7 +5003,7 @@
         <f t="array" ref="H50">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="I50" s="42" t="str">
+      <c r="I50" s="39" t="str">
         <f t="array" ref="I50">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
@@ -4941,7 +5013,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="42" t="str">
+      <c r="B51" s="39" t="str">
         <f t="array" ref="B51">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
@@ -4949,19 +5021,19 @@
         <f t="array" ref="C51">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="D51" s="42" t="str">
+      <c r="D51" s="39" t="str">
         <f t="array" ref="D51">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="E51" s="42" t="str">
+      <c r="E51" s="39" t="str">
         <f t="array" ref="E51">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="F51" s="43" t="str">
+      <c r="F51" s="40" t="str">
         <f t="array" ref="F51">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="G51" s="42" t="str">
+      <c r="G51" s="39" t="str">
         <f t="array" ref="G51">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
@@ -4969,7 +5041,7 @@
         <f t="array" ref="H51">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="I51" s="42" t="str">
+      <c r="I51" s="39" t="str">
         <f t="array" ref="I51">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
@@ -4979,7 +5051,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="42" t="str">
+      <c r="B52" s="39" t="str">
         <f t="array" ref="B52">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
@@ -4987,19 +5059,19 @@
         <f t="array" ref="C52">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="D52" s="42" t="str">
+      <c r="D52" s="39" t="str">
         <f t="array" ref="D52">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="E52" s="42" t="str">
+      <c r="E52" s="39" t="str">
         <f t="array" ref="E52">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="F52" s="43" t="str">
+      <c r="F52" s="40" t="str">
         <f t="array" ref="F52">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="G52" s="42" t="str">
+      <c r="G52" s="39" t="str">
         <f t="array" ref="G52">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
@@ -5007,7 +5079,7 @@
         <f t="array" ref="H52">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="I52" s="42" t="str">
+      <c r="I52" s="39" t="str">
         <f t="array" ref="I52">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
@@ -5017,7 +5089,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="42" t="str">
+      <c r="B53" s="39" t="str">
         <f t="array" ref="B53">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
@@ -5025,19 +5097,19 @@
         <f t="array" ref="C53">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="D53" s="42" t="str">
+      <c r="D53" s="39" t="str">
         <f t="array" ref="D53">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="E53" s="42" t="str">
+      <c r="E53" s="39" t="str">
         <f t="array" ref="E53">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="F53" s="43" t="str">
+      <c r="F53" s="40" t="str">
         <f t="array" ref="F53">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="G53" s="42" t="str">
+      <c r="G53" s="39" t="str">
         <f t="array" ref="G53">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
@@ -5045,7 +5117,7 @@
         <f t="array" ref="H53">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="I53" s="42" t="str">
+      <c r="I53" s="39" t="str">
         <f t="array" ref="I53">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
@@ -5055,7 +5127,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="42" t="str">
+      <c r="B54" s="39" t="str">
         <f t="array" ref="B54">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
@@ -5063,19 +5135,19 @@
         <f t="array" ref="C54">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="D54" s="42" t="str">
+      <c r="D54" s="39" t="str">
         <f t="array" ref="D54">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="E54" s="42" t="str">
+      <c r="E54" s="39" t="str">
         <f t="array" ref="E54">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="F54" s="43" t="str">
+      <c r="F54" s="40" t="str">
         <f t="array" ref="F54">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="G54" s="42" t="str">
+      <c r="G54" s="39" t="str">
         <f t="array" ref="G54">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
@@ -5083,7 +5155,7 @@
         <f t="array" ref="H54">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="I54" s="42" t="str">
+      <c r="I54" s="39" t="str">
         <f t="array" ref="I54">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
@@ -5132,11 +5204,20 @@
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kc1u60ocaBoFYQBZ/9jaT8GKSXPgKCRK+dDFTiZ8J+GtCLKKdu14CtuU8gGM5yGnW2c9mc2/MWq6ELZ2B+AQbw==" saltValue="ldLzTX59WNjU2YCP2uAw9w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
   </mergeCells>
+  <conditionalFormatting sqref="M16:M17">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>$H$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>$H$4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -5151,7 +5232,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5221,7 +5302,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>92.15</v>
+        <v>96.15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
@@ -5738,18 +5819,18 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Atualiza planilha com saldo e formatação condicional
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCCE17B-AC7B-413C-80B7-EB6E16743677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03F8F14-E077-4359-9E9B-039365C58D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
@@ -616,16 +616,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -633,7 +633,14 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="57">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -652,6 +659,97 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2804,34 +2902,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="56">
   <autoFilter ref="B5:J55" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="55">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="40" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="54" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="53">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="52">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="51">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="50">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="49">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="48">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="33" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="47" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2840,35 +2938,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Moeda">
       <calculatedColumnFormula>RANDBETWEEN(150,956)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="22" totalsRowDxfId="21">
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="36" totalsRowDxfId="35">
       <calculatedColumnFormula>RANDBETWEEN(1/8/2025,30/8/2025)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="28" totalsRowDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="7" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="21" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3174,7 +3272,7 @@
   <dimension ref="B1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3710,10 +3808,10 @@
         <f t="array" ref="J16">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="47">
+      <c r="M16" s="49">
         <f>J4-H4</f>
         <v>3944.85</v>
       </c>
@@ -3755,8 +3853,8 @@
         <f t="array" ref="J17">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="L17" s="50"/>
-      <c r="M17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="50"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="39" t="str">
@@ -5211,11 +5309,14 @@
     <mergeCell ref="M16:M17"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
       <formula>$H$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5232,7 +5333,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5819,18 +5920,18 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5854,7 +5955,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Atualiza planilha com proteção, saldo e formatação condicional
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03F8F14-E077-4359-9E9B-039365C58D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDAF717-6713-4DAC-9C03-119C20E085F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
@@ -633,28 +633,7 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="43">
     <dxf>
       <fill>
         <patternFill>
@@ -673,83 +652,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2902,34 +2804,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="B5:J55" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="41">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="54" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="40" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="53">
+    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="39">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="52">
+    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="38">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="51">
+    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="37">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="50">
+    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="36">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="49">
+    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="35">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="48">
+    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="34">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="47" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="33" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2938,35 +2840,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Moeda">
       <calculatedColumnFormula>RANDBETWEEN(150,956)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="36" totalsRowDxfId="35">
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>RANDBETWEEN(1/8/2025,30/8/2025)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="21" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="7" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3272,7 +3174,7 @@
   <dimension ref="B1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5302,6 +5204,7 @@
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="9Vh6T0ztf534Xbtq2lwR6Az4kqhoAhsn0xJc1Ex5HCXAqiHek87viBaRJVPCickCiyQUHTPRjRvoUtgPF95eXA==" saltValue="XDCcdMJskOjPS728pJ49YA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
@@ -5309,13 +5212,13 @@
     <mergeCell ref="M16:M17"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5920,18 +5823,18 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Versão final da planilha: saldo, formatação condicional e proteção
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF79EC0A-0EB6-4378-A569-146DCD8D6B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E941C-2230-4688-9FC1-6FC0484BD9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSULTA" sheetId="20" r:id="rId1"/>
@@ -3173,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D74486-E613-4DD7-8E3C-257D31A44268}">
   <dimension ref="B1:M56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5204,7 +5204,7 @@
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9Vh6T0ztf534Xbtq2lwR6Az4kqhoAhsn0xJc1Ex5HCXAqiHek87viBaRJVPCickCiyQUHTPRjRvoUtgPF95eXA==" saltValue="XDCcdMJskOjPS728pJ49YA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Wy+sCf5SDGRV7DvAHC3zVg7ByMGkKo/KD3jkOHLK8xlQvXcgAdcok0YpcaQaVN5n8kXrNLjj2+yElVmdBzi+TA==" saltValue="51VClw+bZP3v+6hd7/ocbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
@@ -5857,7 +5857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9411D7FE-CD27-49EB-BAB1-5AA613EEF804}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualiza coluna STATUS na planilha
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E941C-2230-4688-9FC1-6FC0484BD9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3DAE31-1499-4862-8DCB-1920DBCCE3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>DESCRIÇÃO</t>
   </si>
@@ -62,31 +62,13 @@
     <t>PAGO</t>
   </si>
   <si>
-    <t>BOLETO</t>
-  </si>
-  <si>
-    <t>DINHEIRO</t>
-  </si>
-  <si>
-    <t>LAZER</t>
-  </si>
-  <si>
     <t>PENDENTE</t>
-  </si>
-  <si>
-    <t>DESPESA</t>
-  </si>
-  <si>
-    <t>RENDIMENTOS</t>
   </si>
   <si>
     <t>MÊS</t>
   </si>
   <si>
     <t>ANO</t>
-  </si>
-  <si>
-    <t>SALÁRIO</t>
   </si>
   <si>
     <t>SAÍDAS</t>
@@ -118,15 +100,6 @@
       </rPr>
       <t>_</t>
     </r>
-  </si>
-  <si>
-    <t>MC DONALDS</t>
-  </si>
-  <si>
-    <t>LUZ</t>
-  </si>
-  <si>
-    <t>ÁGUA</t>
   </si>
   <si>
     <t>SALDO</t>
@@ -633,7 +606,35 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1154,10 +1155,10 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>159.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,10 +1326,10 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>191.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2804,34 +2805,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="B5:J55" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="45">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="40" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="44" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="43">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="42">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="41">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="40">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="39">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="38">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="33" dataCellStyle="Moeda">
+    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="37" dataCellStyle="Moeda">
       <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2840,35 +2841,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Moeda">
-      <calculatedColumnFormula>RANDBETWEEN(150,956)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="22" totalsRowDxfId="21">
-      <calculatedColumnFormula>RANDBETWEEN(1/8/2025,30/8/2025)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="7" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="11" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3200,13 +3197,13 @@
     <row r="1" spans="2:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" s="28">
         <v>8</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F2" s="45"/>
       <c r="G2" s="45"/>
@@ -3215,12 +3212,12 @@
       </c>
       <c r="M2" s="18">
         <f>SUMPRODUCT((R_TABELA[STATUS]=L2)*(MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3)*(R_TABELA[VALOR]))</f>
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" s="28">
         <v>2025</v>
@@ -3229,39 +3226,39 @@
       <c r="F3" s="45"/>
       <c r="G3" s="45"/>
       <c r="I3" s="26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J3" s="27">
         <f>H4</f>
-        <v>191.15</v>
+        <v>0</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M3" s="16">
         <f>SUMPRODUCT((R_TABELA[STATUS]=L3)*(MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3)*(R_TABELA[VALOR]))</f>
-        <v>159.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23"/>
       <c r="C4" s="35"/>
       <c r="D4" s="46" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
       <c r="G4" s="46"/>
       <c r="H4" s="44">
         <f>SUM(C6:C55)</f>
-        <v>191.15</v>
+        <v>0</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J4" s="43">
         <f>SUM(J6:J55)</f>
-        <v>4136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3287,116 +3284,116 @@
         <v>6</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="str">
         <f t="array" ref="B6">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
-        <v>MC DONALDS</v>
-      </c>
-      <c r="C6" s="30">
+        <v/>
+      </c>
+      <c r="C6" s="30" t="str">
         <f t="array" ref="C6">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</f>
-        <v>32</v>
+        <v/>
       </c>
       <c r="D6" s="29" t="str">
         <f t="array" ref="D6">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</f>
-        <v>PAGO</v>
+        <v/>
       </c>
       <c r="E6" s="29" t="str">
         <f t="array" ref="E6">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</f>
-        <v>LAZER</v>
-      </c>
-      <c r="F6" s="31">
+        <v/>
+      </c>
+      <c r="F6" s="31" t="str">
         <f t="array" ref="F6">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</f>
-        <v>45886</v>
+        <v/>
       </c>
       <c r="G6" s="29" t="str">
         <f t="array" ref="G6">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</f>
-        <v>DINHEIRO</v>
-      </c>
-      <c r="H6" s="32">
+        <v/>
+      </c>
+      <c r="H6" s="32" t="str">
         <f t="array" ref="H6">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I6" s="29" t="str">
         <f t="array" ref="I6">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
-        <v>SALÁRIO</v>
-      </c>
-      <c r="J6" s="30">
+        <v/>
+      </c>
+      <c r="J6" s="30" t="str">
         <f t="array" ref="J6">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</f>
-        <v>3900</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="39" t="str">
         <f t="array" ref="B7">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
-        <v>LUZ</v>
-      </c>
-      <c r="C7" s="19">
+        <v/>
+      </c>
+      <c r="C7" s="19" t="str">
         <f t="array" ref="C7">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(2:2))),"")</f>
-        <v>96.15</v>
+        <v/>
       </c>
       <c r="D7" s="39" t="str">
         <f t="array" ref="D7">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(2:2))),"")</f>
-        <v>PENDENTE</v>
+        <v/>
       </c>
       <c r="E7" s="39" t="str">
         <f t="array" ref="E7">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(2:2))),"")</f>
-        <v>DESPESA</v>
-      </c>
-      <c r="F7" s="40">
+        <v/>
+      </c>
+      <c r="F7" s="40" t="str">
         <f t="array" ref="F7">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(2:2))),"")</f>
-        <v>45891</v>
+        <v/>
       </c>
       <c r="G7" s="39" t="str">
         <f t="array" ref="G7">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(2:2))),"")</f>
-        <v>BOLETO</v>
-      </c>
-      <c r="H7" s="33">
+        <v/>
+      </c>
+      <c r="H7" s="33" t="str">
         <f t="array" ref="H7">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(2:2))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I7" s="39" t="str">
         <f t="array" ref="I7">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
-        <v>RENDIMENTOS</v>
-      </c>
-      <c r="J7" s="19">
+        <v/>
+      </c>
+      <c r="J7" s="19" t="str">
         <f t="array" ref="J7">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(2:2))),"")</f>
-        <v>236</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="39" t="str">
         <f t="array" ref="B8">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
-        <v>ÁGUA</v>
-      </c>
-      <c r="C8" s="19">
+        <v/>
+      </c>
+      <c r="C8" s="19" t="str">
         <f t="array" ref="C8">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(3:3))),"")</f>
-        <v>63</v>
+        <v/>
       </c>
       <c r="D8" s="39" t="str">
         <f t="array" ref="D8">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(3:3))),"")</f>
-        <v>PENDENTE</v>
+        <v/>
       </c>
       <c r="E8" s="39" t="str">
         <f t="array" ref="E8">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(3:3))),"")</f>
-        <v>DESPESA</v>
-      </c>
-      <c r="F8" s="40">
+        <v/>
+      </c>
+      <c r="F8" s="40" t="str">
         <f t="array" ref="F8">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(3:3))),"")</f>
-        <v>45891</v>
+        <v/>
       </c>
       <c r="G8" s="39" t="str">
         <f t="array" ref="G8">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(3:3))),"")</f>
-        <v>BOLETO</v>
-      </c>
-      <c r="H8" s="33">
+        <v/>
+      </c>
+      <c r="H8" s="33" t="str">
         <f t="array" ref="H8">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(3:3))),"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="I8" s="39" t="str">
         <f t="array" ref="I8">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
@@ -3711,11 +3708,11 @@
         <v/>
       </c>
       <c r="L16" s="47" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M16" s="49">
         <f>J4-H4</f>
-        <v>3944.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5204,7 +5201,7 @@
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Wy+sCf5SDGRV7DvAHC3zVg7ByMGkKo/KD3jkOHLK8xlQvXcgAdcok0YpcaQaVN5n8kXrNLjj2+yElVmdBzi+TA==" saltValue="51VClw+bZP3v+6hd7/ocbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rHWjBQR5Qqic9iItYVKaQP4eg7hzOXsWAsZiPyKZF0omAXyW/Rxf2qICdVJmT7R18/K7tUtdff9QbmcJkCoCtg==" saltValue="EkExKNYtiZ3w5hp17N3KlA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
@@ -5212,13 +5209,13 @@
     <mergeCell ref="M16:M17"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThanOrEqual">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>$H$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5236,7 +5233,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5282,64 +5279,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="1">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3">
-        <v>45886</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1">
-        <v>96.15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3">
-        <v>45891</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1">
-        <v>63</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3">
-        <v>45891</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
@@ -5822,19 +5768,33 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="C1:C161">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C161">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"PAGO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C162:C1048576">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"INVESTIMENTO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"PARCELADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"PENDENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5842,7 +5802,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C162:C1048576" xr:uid="{8F5598F2-1887-4907-A141-5ACA1B7011F5}">
       <formula1>"PAGO,PENDENTE,PARCELADO,INVESTIMENTO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C161" xr:uid="{A446CFE5-5D16-4310-AE4A-3EC37E3DC262}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C161" xr:uid="{2922D9E2-37F4-49CA-A6CF-FFA4850A6792}">
       <formula1>"PAGO,PENDENTE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5855,10 +5815,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9411D7FE-CD27-49EB-BAB1-5AA613EEF804}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5872,44 +5832,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="8">
-        <v>3900</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="8">
-        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização da planilha financeira
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E19A420-94AB-4DCC-9D87-FE7D2E504480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7635C129-411D-4C17-8CE9-2FE31DAD5AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSULTA" sheetId="20" r:id="rId1"/>
@@ -145,14 +145,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="25"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,6 +168,14 @@
       <b/>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -306,15 +306,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -331,15 +322,6 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -401,17 +383,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -445,12 +416,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -477,25 +562,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,109 +589,184 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -709,10 +869,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -836,155 +992,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2678,61 +2685,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="184731" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4BBC3FE-08EA-B661-F6F6-6039C0350EF7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4171950" y="2428875"/>
-          <a:ext cx="184731" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2805,67 +2757,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}" name="Tabela3" displayName="Tabela3" ref="B5:J55" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="B5:J55" xr:uid="{53E94832-4332-43EE-9835-717F7E76CAA1}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{37C207DB-3392-4539-88F1-FF4A619D7214}" name="DESCRIÇÃO" dataDxfId="45">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{69001C81-3CC8-4304-9771-BFA7E0FBBF5D}" name="VALOR" dataDxfId="44" dataCellStyle="Moeda">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{492B8990-9E2C-4071-BD50-D1ED9FB55077}" name="STATUS" dataDxfId="43">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{EA8B9AA5-0430-4BE4-92EE-C98A706513E8}" name="CATEGORIA" dataDxfId="42">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5F99F89-2F30-4042-BE76-5D5095EC6FAD}" name="DATA DE VENCIMENTO" dataDxfId="41">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{28766BEE-68A6-495F-A303-3495417A4438}" name="FORMA DE PAGAMENTO" dataDxfId="40">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{17D98CC8-9C87-454E-A341-8405CA11B93D}" name="PARCELA" dataDxfId="39">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{F7CA1604-A9B5-46BA-A770-A26D1DC6F417}" name="DESCRIÇÃO_" dataDxfId="38">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{2A9A3637-D94D-41D8-954A-C01A414AAF69}" name="VALOR(R$)" dataDxfId="37" dataCellStyle="Moeda">
-      <calculatedColumnFormula array="1">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="4" totalsRowDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="11" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="20" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3170,28 +3086,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D74486-E613-4DD7-8E3C-257D31A44268}">
   <dimension ref="B1:M56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" style="23" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="23"/>
-    <col min="15" max="15" width="12.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="1.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="19"/>
+    <col min="15" max="15" width="12.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3199,14 +3115,14 @@
       <c r="B2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="24">
         <v>8</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
       <c r="L2" s="17" t="s">
         <v>9</v>
       </c>
@@ -3219,16 +3135,16 @@
       <c r="B3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="24">
         <v>2025</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="I3" s="26" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="I3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="23">
         <f>H4</f>
         <v>0</v>
       </c>
@@ -3241,1967 +3157,1966 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="46" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="44">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="27">
         <f>SUM(C6:C55)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="26">
         <f>SUM(J6:J55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="37" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="str">
+      <c r="B6" s="38" t="str">
         <f t="array" ref="B6">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="C6" s="30" t="str">
+      <c r="C6" s="39" t="str">
         <f t="array" ref="C6">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="D6" s="29" t="str">
+      <c r="D6" s="40" t="str">
         <f t="array" ref="D6">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="E6" s="29" t="str">
+      <c r="E6" s="40" t="str">
         <f t="array" ref="E6">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="F6" s="31" t="str">
+      <c r="F6" s="41" t="str">
         <f t="array" ref="F6">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="G6" s="29" t="str">
+      <c r="G6" s="40" t="str">
         <f t="array" ref="G6">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="H6" s="32" t="str">
+      <c r="H6" s="40" t="str">
         <f t="array" ref="H6">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="I6" s="29" t="str">
+      <c r="I6" s="42" t="str">
         <f t="array" ref="I6">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="J6" s="30" t="str">
+      <c r="J6" s="43" t="str">
         <f t="array" ref="J6">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="str">
+      <c r="B7" s="44" t="str">
         <f t="array" ref="B7">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="C7" s="19" t="str">
+      <c r="C7" s="45" t="str">
         <f t="array" ref="C7">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="D7" s="39" t="str">
+      <c r="D7" s="46" t="str">
         <f t="array" ref="D7">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="E7" s="39" t="str">
+      <c r="E7" s="46" t="str">
         <f t="array" ref="E7">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="F7" s="40" t="str">
+      <c r="F7" s="47" t="str">
         <f t="array" ref="F7">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="G7" s="39" t="str">
+      <c r="G7" s="46" t="str">
         <f t="array" ref="G7">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="H7" s="33" t="str">
+      <c r="H7" s="46" t="str">
         <f t="array" ref="H7">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="I7" s="39" t="str">
+      <c r="I7" s="48" t="str">
         <f t="array" ref="I7">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="J7" s="19" t="str">
+      <c r="J7" s="49" t="str">
         <f t="array" ref="J7">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="str">
+      <c r="B8" s="44" t="str">
         <f t="array" ref="B8">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="C8" s="19" t="str">
+      <c r="C8" s="45" t="str">
         <f t="array" ref="C8">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="D8" s="39" t="str">
+      <c r="D8" s="46" t="str">
         <f t="array" ref="D8">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="E8" s="39" t="str">
+      <c r="E8" s="46" t="str">
         <f t="array" ref="E8">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="F8" s="40" t="str">
+      <c r="F8" s="47" t="str">
         <f t="array" ref="F8">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="G8" s="39" t="str">
+      <c r="G8" s="46" t="str">
         <f t="array" ref="G8">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="H8" s="33" t="str">
+      <c r="H8" s="46" t="str">
         <f t="array" ref="H8">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="I8" s="39" t="str">
+      <c r="I8" s="48" t="str">
         <f t="array" ref="I8">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="J8" s="19" t="str">
+      <c r="J8" s="49" t="str">
         <f t="array" ref="J8">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="str">
+      <c r="B9" s="44" t="str">
         <f t="array" ref="B9">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="C9" s="19" t="str">
+      <c r="C9" s="45" t="str">
         <f t="array" ref="C9">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="D9" s="39" t="str">
+      <c r="D9" s="46" t="str">
         <f t="array" ref="D9">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="E9" s="39" t="str">
+      <c r="E9" s="46" t="str">
         <f t="array" ref="E9">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="F9" s="40" t="str">
+      <c r="F9" s="47" t="str">
         <f t="array" ref="F9">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="G9" s="39" t="str">
+      <c r="G9" s="46" t="str">
         <f t="array" ref="G9">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="H9" s="33" t="str">
+      <c r="H9" s="46" t="str">
         <f t="array" ref="H9">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="I9" s="39" t="str">
+      <c r="I9" s="48" t="str">
         <f t="array" ref="I9">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="J9" s="19" t="str">
+      <c r="J9" s="49" t="str">
         <f t="array" ref="J9">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="str">
+      <c r="B10" s="44" t="str">
         <f t="array" ref="B10">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="C10" s="19" t="str">
+      <c r="C10" s="45" t="str">
         <f t="array" ref="C10">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="D10" s="39" t="str">
+      <c r="D10" s="46" t="str">
         <f t="array" ref="D10">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="E10" s="39" t="str">
+      <c r="E10" s="46" t="str">
         <f t="array" ref="E10">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="F10" s="40" t="str">
+      <c r="F10" s="47" t="str">
         <f t="array" ref="F10">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="G10" s="39" t="str">
+      <c r="G10" s="46" t="str">
         <f t="array" ref="G10">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="H10" s="33" t="str">
+      <c r="H10" s="46" t="str">
         <f t="array" ref="H10">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="I10" s="39" t="str">
+      <c r="I10" s="48" t="str">
         <f t="array" ref="I10">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="J10" s="19" t="str">
+      <c r="J10" s="49" t="str">
         <f t="array" ref="J10">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="str">
+      <c r="B11" s="44" t="str">
         <f t="array" ref="B11">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="45" t="str">
         <f t="array" ref="C11">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="D11" s="39" t="str">
+      <c r="D11" s="46" t="str">
         <f t="array" ref="D11">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="E11" s="39" t="str">
+      <c r="E11" s="46" t="str">
         <f t="array" ref="E11">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="F11" s="40" t="str">
+      <c r="F11" s="47" t="str">
         <f t="array" ref="F11">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="G11" s="39" t="str">
+      <c r="G11" s="46" t="str">
         <f t="array" ref="G11">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="H11" s="33" t="str">
+      <c r="H11" s="46" t="str">
         <f t="array" ref="H11">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="I11" s="39" t="str">
+      <c r="I11" s="48" t="str">
         <f t="array" ref="I11">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="J11" s="19" t="str">
+      <c r="J11" s="49" t="str">
         <f t="array" ref="J11">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="str">
+      <c r="B12" s="44" t="str">
         <f t="array" ref="B12">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="45" t="str">
         <f t="array" ref="C12">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="D12" s="39" t="str">
+      <c r="D12" s="46" t="str">
         <f t="array" ref="D12">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="E12" s="39" t="str">
+      <c r="E12" s="46" t="str">
         <f t="array" ref="E12">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="F12" s="40" t="str">
+      <c r="F12" s="47" t="str">
         <f t="array" ref="F12">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="G12" s="39" t="str">
+      <c r="G12" s="46" t="str">
         <f t="array" ref="G12">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="H12" s="33" t="str">
+      <c r="H12" s="46" t="str">
         <f t="array" ref="H12">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="I12" s="39" t="str">
+      <c r="I12" s="48" t="str">
         <f t="array" ref="I12">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="J12" s="19" t="str">
+      <c r="J12" s="49" t="str">
         <f t="array" ref="J12">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="str">
+      <c r="B13" s="44" t="str">
         <f t="array" ref="B13">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="C13" s="19" t="str">
+      <c r="C13" s="45" t="str">
         <f t="array" ref="C13">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="D13" s="39" t="str">
+      <c r="D13" s="46" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="E13" s="39" t="str">
+      <c r="E13" s="46" t="str">
         <f t="array" ref="E13">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="F13" s="40" t="str">
+      <c r="F13" s="47" t="str">
         <f t="array" ref="F13">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="G13" s="39" t="str">
+      <c r="G13" s="46" t="str">
         <f t="array" ref="G13">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="H13" s="33" t="str">
+      <c r="H13" s="46" t="str">
         <f t="array" ref="H13">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="I13" s="39" t="str">
+      <c r="I13" s="48" t="str">
         <f t="array" ref="I13">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="J13" s="19" t="str">
+      <c r="J13" s="49" t="str">
         <f t="array" ref="J13">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="str">
+      <c r="B14" s="44" t="str">
         <f t="array" ref="B14">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="C14" s="19" t="str">
+      <c r="C14" s="45" t="str">
         <f t="array" ref="C14">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="D14" s="39" t="str">
+      <c r="D14" s="46" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="E14" s="39" t="str">
+      <c r="E14" s="46" t="str">
         <f t="array" ref="E14">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="F14" s="40" t="str">
+      <c r="F14" s="47" t="str">
         <f t="array" ref="F14">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="G14" s="39" t="str">
+      <c r="G14" s="46" t="str">
         <f t="array" ref="G14">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="H14" s="33" t="str">
+      <c r="H14" s="46" t="str">
         <f t="array" ref="H14">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="I14" s="39" t="str">
+      <c r="I14" s="48" t="str">
         <f t="array" ref="I14">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="J14" s="19" t="str">
+      <c r="J14" s="49" t="str">
         <f t="array" ref="J14">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="39" t="str">
+      <c r="B15" s="44" t="str">
         <f t="array" ref="B15">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="C15" s="19" t="str">
+      <c r="C15" s="45" t="str">
         <f t="array" ref="C15">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="D15" s="39" t="str">
+      <c r="D15" s="46" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="E15" s="39" t="str">
+      <c r="E15" s="46" t="str">
         <f t="array" ref="E15">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="F15" s="40" t="str">
+      <c r="F15" s="47" t="str">
         <f t="array" ref="F15">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="G15" s="39" t="str">
+      <c r="G15" s="46" t="str">
         <f t="array" ref="G15">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="H15" s="33" t="str">
+      <c r="H15" s="46" t="str">
         <f t="array" ref="H15">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="I15" s="39" t="str">
+      <c r="I15" s="48" t="str">
         <f t="array" ref="I15">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="J15" s="19" t="str">
+      <c r="J15" s="49" t="str">
         <f t="array" ref="J15">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="str">
+      <c r="B16" s="44" t="str">
         <f t="array" ref="B16">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="C16" s="19" t="str">
+      <c r="C16" s="45" t="str">
         <f t="array" ref="C16">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="D16" s="39" t="str">
+      <c r="D16" s="46" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="E16" s="39" t="str">
+      <c r="E16" s="46" t="str">
         <f t="array" ref="E16">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="F16" s="40" t="str">
+      <c r="F16" s="47" t="str">
         <f t="array" ref="F16">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="G16" s="39" t="str">
+      <c r="G16" s="46" t="str">
         <f t="array" ref="G16">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="H16" s="33" t="str">
+      <c r="H16" s="46" t="str">
         <f t="array" ref="H16">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="I16" s="39" t="str">
+      <c r="I16" s="48" t="str">
         <f t="array" ref="I16">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="J16" s="19" t="str">
+      <c r="J16" s="49" t="str">
         <f t="array" ref="J16">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="L16" s="47" t="s">
+      <c r="L16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="49">
+      <c r="M16" s="32">
         <f>J4-H4</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="39" t="str">
+      <c r="B17" s="44" t="str">
         <f t="array" ref="B17">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="C17" s="19" t="str">
+      <c r="C17" s="45" t="str">
         <f t="array" ref="C17">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="D17" s="39" t="str">
+      <c r="D17" s="46" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="E17" s="39" t="str">
+      <c r="E17" s="46" t="str">
         <f t="array" ref="E17">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="F17" s="40" t="str">
+      <c r="F17" s="47" t="str">
         <f t="array" ref="F17">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="G17" s="39" t="str">
+      <c r="G17" s="46" t="str">
         <f t="array" ref="G17">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="H17" s="33" t="str">
+      <c r="H17" s="46" t="str">
         <f t="array" ref="H17">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="I17" s="39" t="str">
+      <c r="I17" s="48" t="str">
         <f t="array" ref="I17">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="J17" s="19" t="str">
+      <c r="J17" s="49" t="str">
         <f t="array" ref="J17">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="50"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="39" t="str">
+      <c r="B18" s="44" t="str">
         <f t="array" ref="B18">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="C18" s="19" t="str">
+      <c r="C18" s="45" t="str">
         <f t="array" ref="C18">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="D18" s="39" t="str">
+      <c r="D18" s="46" t="str">
         <f t="array" ref="D18">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="E18" s="39" t="str">
+      <c r="E18" s="46" t="str">
         <f t="array" ref="E18">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="F18" s="40" t="str">
+      <c r="F18" s="47" t="str">
         <f t="array" ref="F18">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="G18" s="39" t="str">
+      <c r="G18" s="46" t="str">
         <f t="array" ref="G18">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="H18" s="33" t="str">
+      <c r="H18" s="46" t="str">
         <f t="array" ref="H18">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="I18" s="39" t="str">
+      <c r="I18" s="48" t="str">
         <f t="array" ref="I18">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="J18" s="19" t="str">
+      <c r="J18" s="49" t="str">
         <f t="array" ref="J18">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="39" t="str">
+      <c r="B19" s="44" t="str">
         <f t="array" ref="B19">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="C19" s="19" t="str">
+      <c r="C19" s="45" t="str">
         <f t="array" ref="C19">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="D19" s="39" t="str">
+      <c r="D19" s="46" t="str">
         <f t="array" ref="D19">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="E19" s="39" t="str">
+      <c r="E19" s="46" t="str">
         <f t="array" ref="E19">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="F19" s="40" t="str">
+      <c r="F19" s="47" t="str">
         <f t="array" ref="F19">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="G19" s="39" t="str">
+      <c r="G19" s="46" t="str">
         <f t="array" ref="G19">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="H19" s="33" t="str">
+      <c r="H19" s="46" t="str">
         <f t="array" ref="H19">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="I19" s="39" t="str">
+      <c r="I19" s="48" t="str">
         <f t="array" ref="I19">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="J19" s="19" t="str">
+      <c r="J19" s="49" t="str">
         <f t="array" ref="J19">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="str">
+      <c r="B20" s="44" t="str">
         <f t="array" ref="B20">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="C20" s="19" t="str">
+      <c r="C20" s="45" t="str">
         <f t="array" ref="C20">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="D20" s="39" t="str">
+      <c r="D20" s="46" t="str">
         <f t="array" ref="D20">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="E20" s="39" t="str">
+      <c r="E20" s="46" t="str">
         <f t="array" ref="E20">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="F20" s="40" t="str">
+      <c r="F20" s="47" t="str">
         <f t="array" ref="F20">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="G20" s="39" t="str">
+      <c r="G20" s="46" t="str">
         <f t="array" ref="G20">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="H20" s="33" t="str">
+      <c r="H20" s="46" t="str">
         <f t="array" ref="H20">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="I20" s="39" t="str">
+      <c r="I20" s="48" t="str">
         <f t="array" ref="I20">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="J20" s="19" t="str">
+      <c r="J20" s="49" t="str">
         <f t="array" ref="J20">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="39" t="str">
+      <c r="B21" s="44" t="str">
         <f t="array" ref="B21">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="C21" s="19" t="str">
+      <c r="C21" s="45" t="str">
         <f t="array" ref="C21">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="D21" s="39" t="str">
+      <c r="D21" s="46" t="str">
         <f t="array" ref="D21">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="E21" s="39" t="str">
+      <c r="E21" s="46" t="str">
         <f t="array" ref="E21">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="F21" s="40" t="str">
+      <c r="F21" s="47" t="str">
         <f t="array" ref="F21">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="G21" s="39" t="str">
+      <c r="G21" s="46" t="str">
         <f t="array" ref="G21">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="H21" s="33" t="str">
+      <c r="H21" s="46" t="str">
         <f t="array" ref="H21">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="I21" s="39" t="str">
+      <c r="I21" s="48" t="str">
         <f t="array" ref="I21">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="J21" s="19" t="str">
+      <c r="J21" s="49" t="str">
         <f t="array" ref="J21">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="39" t="str">
+      <c r="B22" s="44" t="str">
         <f t="array" ref="B22">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="C22" s="19" t="str">
+      <c r="C22" s="45" t="str">
         <f t="array" ref="C22">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="D22" s="39" t="str">
+      <c r="D22" s="46" t="str">
         <f t="array" ref="D22">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="E22" s="39" t="str">
+      <c r="E22" s="46" t="str">
         <f t="array" ref="E22">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="F22" s="40" t="str">
+      <c r="F22" s="47" t="str">
         <f t="array" ref="F22">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="G22" s="39" t="str">
+      <c r="G22" s="46" t="str">
         <f t="array" ref="G22">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="H22" s="33" t="str">
+      <c r="H22" s="46" t="str">
         <f t="array" ref="H22">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="I22" s="39" t="str">
+      <c r="I22" s="48" t="str">
         <f t="array" ref="I22">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="J22" s="19" t="str">
+      <c r="J22" s="49" t="str">
         <f t="array" ref="J22">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="str">
+      <c r="B23" s="44" t="str">
         <f t="array" ref="B23">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="C23" s="19" t="str">
+      <c r="C23" s="45" t="str">
         <f t="array" ref="C23">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="D23" s="39" t="str">
+      <c r="D23" s="46" t="str">
         <f t="array" ref="D23">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="E23" s="39" t="str">
+      <c r="E23" s="46" t="str">
         <f t="array" ref="E23">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="F23" s="40" t="str">
+      <c r="F23" s="47" t="str">
         <f t="array" ref="F23">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="G23" s="39" t="str">
+      <c r="G23" s="46" t="str">
         <f t="array" ref="G23">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="H23" s="33" t="str">
+      <c r="H23" s="46" t="str">
         <f t="array" ref="H23">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="I23" s="39" t="str">
+      <c r="I23" s="48" t="str">
         <f t="array" ref="I23">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="J23" s="19" t="str">
+      <c r="J23" s="49" t="str">
         <f t="array" ref="J23">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="str">
+      <c r="B24" s="44" t="str">
         <f t="array" ref="B24">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="C24" s="19" t="str">
+      <c r="C24" s="45" t="str">
         <f t="array" ref="C24">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="D24" s="39" t="str">
+      <c r="D24" s="46" t="str">
         <f t="array" ref="D24">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="E24" s="39" t="str">
+      <c r="E24" s="46" t="str">
         <f t="array" ref="E24">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="F24" s="40" t="str">
+      <c r="F24" s="47" t="str">
         <f t="array" ref="F24">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="G24" s="39" t="str">
+      <c r="G24" s="46" t="str">
         <f t="array" ref="G24">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="H24" s="33" t="str">
+      <c r="H24" s="46" t="str">
         <f t="array" ref="H24">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="I24" s="39" t="str">
+      <c r="I24" s="48" t="str">
         <f t="array" ref="I24">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="J24" s="19" t="str">
+      <c r="J24" s="49" t="str">
         <f t="array" ref="J24">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="str">
+      <c r="B25" s="44" t="str">
         <f t="array" ref="B25">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="C25" s="19" t="str">
+      <c r="C25" s="45" t="str">
         <f t="array" ref="C25">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="D25" s="39" t="str">
+      <c r="D25" s="46" t="str">
         <f t="array" ref="D25">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="E25" s="39" t="str">
+      <c r="E25" s="46" t="str">
         <f t="array" ref="E25">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="F25" s="40" t="str">
+      <c r="F25" s="47" t="str">
         <f t="array" ref="F25">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="G25" s="39" t="str">
+      <c r="G25" s="46" t="str">
         <f t="array" ref="G25">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="H25" s="33" t="str">
+      <c r="H25" s="46" t="str">
         <f t="array" ref="H25">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="I25" s="39" t="str">
+      <c r="I25" s="48" t="str">
         <f t="array" ref="I25">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="J25" s="19" t="str">
+      <c r="J25" s="49" t="str">
         <f t="array" ref="J25">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="str">
+      <c r="B26" s="44" t="str">
         <f t="array" ref="B26">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="C26" s="19" t="str">
+      <c r="C26" s="45" t="str">
         <f t="array" ref="C26">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="D26" s="39" t="str">
+      <c r="D26" s="46" t="str">
         <f t="array" ref="D26">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="E26" s="39" t="str">
+      <c r="E26" s="46" t="str">
         <f t="array" ref="E26">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="F26" s="40" t="str">
+      <c r="F26" s="47" t="str">
         <f t="array" ref="F26">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="G26" s="39" t="str">
+      <c r="G26" s="46" t="str">
         <f t="array" ref="G26">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="H26" s="33" t="str">
+      <c r="H26" s="46" t="str">
         <f t="array" ref="H26">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="I26" s="39" t="str">
+      <c r="I26" s="48" t="str">
         <f t="array" ref="I26">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="J26" s="19" t="str">
+      <c r="J26" s="49" t="str">
         <f t="array" ref="J26">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="str">
+      <c r="B27" s="44" t="str">
         <f t="array" ref="B27">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="C27" s="19" t="str">
+      <c r="C27" s="45" t="str">
         <f t="array" ref="C27">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="D27" s="39" t="str">
+      <c r="D27" s="46" t="str">
         <f t="array" ref="D27">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="E27" s="39" t="str">
+      <c r="E27" s="46" t="str">
         <f t="array" ref="E27">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="F27" s="40" t="str">
+      <c r="F27" s="47" t="str">
         <f t="array" ref="F27">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="G27" s="39" t="str">
+      <c r="G27" s="46" t="str">
         <f t="array" ref="G27">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="H27" s="33" t="str">
+      <c r="H27" s="46" t="str">
         <f t="array" ref="H27">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="I27" s="39" t="str">
+      <c r="I27" s="48" t="str">
         <f t="array" ref="I27">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="J27" s="19" t="str">
+      <c r="J27" s="49" t="str">
         <f t="array" ref="J27">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="39" t="str">
+      <c r="B28" s="44" t="str">
         <f t="array" ref="B28">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="C28" s="19" t="str">
+      <c r="C28" s="45" t="str">
         <f t="array" ref="C28">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="D28" s="39" t="str">
+      <c r="D28" s="46" t="str">
         <f t="array" ref="D28">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="E28" s="39" t="str">
+      <c r="E28" s="46" t="str">
         <f t="array" ref="E28">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="F28" s="40" t="str">
+      <c r="F28" s="47" t="str">
         <f t="array" ref="F28">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="G28" s="39" t="str">
+      <c r="G28" s="46" t="str">
         <f t="array" ref="G28">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="H28" s="33" t="str">
+      <c r="H28" s="46" t="str">
         <f t="array" ref="H28">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="I28" s="39" t="str">
+      <c r="I28" s="48" t="str">
         <f t="array" ref="I28">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="J28" s="19" t="str">
+      <c r="J28" s="49" t="str">
         <f t="array" ref="J28">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="str">
+      <c r="B29" s="44" t="str">
         <f t="array" ref="B29">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="C29" s="19" t="str">
+      <c r="C29" s="45" t="str">
         <f t="array" ref="C29">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="D29" s="39" t="str">
+      <c r="D29" s="46" t="str">
         <f t="array" ref="D29">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="E29" s="39" t="str">
+      <c r="E29" s="46" t="str">
         <f t="array" ref="E29">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="F29" s="40" t="str">
+      <c r="F29" s="47" t="str">
         <f t="array" ref="F29">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="G29" s="39" t="str">
+      <c r="G29" s="46" t="str">
         <f t="array" ref="G29">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="H29" s="33" t="str">
+      <c r="H29" s="46" t="str">
         <f t="array" ref="H29">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="I29" s="39" t="str">
+      <c r="I29" s="48" t="str">
         <f t="array" ref="I29">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="J29" s="19" t="str">
+      <c r="J29" s="49" t="str">
         <f t="array" ref="J29">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="39" t="str">
+      <c r="B30" s="44" t="str">
         <f t="array" ref="B30">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="C30" s="19" t="str">
+      <c r="C30" s="45" t="str">
         <f t="array" ref="C30">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="D30" s="39" t="str">
+      <c r="D30" s="46" t="str">
         <f t="array" ref="D30">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="E30" s="39" t="str">
+      <c r="E30" s="46" t="str">
         <f t="array" ref="E30">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="F30" s="40" t="str">
+      <c r="F30" s="47" t="str">
         <f t="array" ref="F30">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="G30" s="39" t="str">
+      <c r="G30" s="46" t="str">
         <f t="array" ref="G30">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="H30" s="33" t="str">
+      <c r="H30" s="46" t="str">
         <f t="array" ref="H30">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="I30" s="39" t="str">
+      <c r="I30" s="48" t="str">
         <f t="array" ref="I30">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="J30" s="19" t="str">
+      <c r="J30" s="49" t="str">
         <f t="array" ref="J30">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="39" t="str">
+      <c r="B31" s="44" t="str">
         <f t="array" ref="B31">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="C31" s="19" t="str">
+      <c r="C31" s="45" t="str">
         <f t="array" ref="C31">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="D31" s="39" t="str">
+      <c r="D31" s="46" t="str">
         <f t="array" ref="D31">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="E31" s="39" t="str">
+      <c r="E31" s="46" t="str">
         <f t="array" ref="E31">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="F31" s="40" t="str">
+      <c r="F31" s="47" t="str">
         <f t="array" ref="F31">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="G31" s="39" t="str">
+      <c r="G31" s="46" t="str">
         <f t="array" ref="G31">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="H31" s="33" t="str">
+      <c r="H31" s="46" t="str">
         <f t="array" ref="H31">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="I31" s="39" t="str">
+      <c r="I31" s="48" t="str">
         <f t="array" ref="I31">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="J31" s="19" t="str">
+      <c r="J31" s="49" t="str">
         <f t="array" ref="J31">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="39" t="str">
+      <c r="B32" s="44" t="str">
         <f t="array" ref="B32">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="C32" s="19" t="str">
+      <c r="C32" s="45" t="str">
         <f t="array" ref="C32">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="D32" s="39" t="str">
+      <c r="D32" s="46" t="str">
         <f t="array" ref="D32">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="E32" s="39" t="str">
+      <c r="E32" s="46" t="str">
         <f t="array" ref="E32">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="F32" s="40" t="str">
+      <c r="F32" s="47" t="str">
         <f t="array" ref="F32">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="G32" s="39" t="str">
+      <c r="G32" s="46" t="str">
         <f t="array" ref="G32">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="H32" s="33" t="str">
+      <c r="H32" s="46" t="str">
         <f t="array" ref="H32">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="I32" s="39" t="str">
+      <c r="I32" s="48" t="str">
         <f t="array" ref="I32">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="J32" s="19" t="str">
+      <c r="J32" s="49" t="str">
         <f t="array" ref="J32">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="39" t="str">
+      <c r="B33" s="44" t="str">
         <f t="array" ref="B33">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="C33" s="19" t="str">
+      <c r="C33" s="45" t="str">
         <f t="array" ref="C33">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="D33" s="39" t="str">
+      <c r="D33" s="46" t="str">
         <f t="array" ref="D33">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="E33" s="39" t="str">
+      <c r="E33" s="46" t="str">
         <f t="array" ref="E33">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="F33" s="40" t="str">
+      <c r="F33" s="47" t="str">
         <f t="array" ref="F33">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="G33" s="39" t="str">
+      <c r="G33" s="46" t="str">
         <f t="array" ref="G33">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="H33" s="33" t="str">
+      <c r="H33" s="46" t="str">
         <f t="array" ref="H33">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="I33" s="39" t="str">
+      <c r="I33" s="48" t="str">
         <f t="array" ref="I33">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="J33" s="19" t="str">
+      <c r="J33" s="49" t="str">
         <f t="array" ref="J33">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="39" t="str">
+      <c r="B34" s="44" t="str">
         <f t="array" ref="B34">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="C34" s="19" t="str">
+      <c r="C34" s="45" t="str">
         <f t="array" ref="C34">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="D34" s="39" t="str">
+      <c r="D34" s="46" t="str">
         <f t="array" ref="D34">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="E34" s="39" t="str">
+      <c r="E34" s="46" t="str">
         <f t="array" ref="E34">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="F34" s="40" t="str">
+      <c r="F34" s="47" t="str">
         <f t="array" ref="F34">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="G34" s="39" t="str">
+      <c r="G34" s="46" t="str">
         <f t="array" ref="G34">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="H34" s="33" t="str">
+      <c r="H34" s="46" t="str">
         <f t="array" ref="H34">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="I34" s="39" t="str">
+      <c r="I34" s="48" t="str">
         <f t="array" ref="I34">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="J34" s="19" t="str">
+      <c r="J34" s="49" t="str">
         <f t="array" ref="J34">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="39" t="str">
+      <c r="B35" s="44" t="str">
         <f t="array" ref="B35">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="C35" s="19" t="str">
+      <c r="C35" s="45" t="str">
         <f t="array" ref="C35">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="D35" s="39" t="str">
+      <c r="D35" s="46" t="str">
         <f t="array" ref="D35">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="E35" s="39" t="str">
+      <c r="E35" s="46" t="str">
         <f t="array" ref="E35">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="F35" s="40" t="str">
+      <c r="F35" s="47" t="str">
         <f t="array" ref="F35">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="G35" s="39" t="str">
+      <c r="G35" s="46" t="str">
         <f t="array" ref="G35">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="H35" s="33" t="str">
+      <c r="H35" s="46" t="str">
         <f t="array" ref="H35">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="I35" s="39" t="str">
+      <c r="I35" s="48" t="str">
         <f t="array" ref="I35">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="J35" s="19" t="str">
+      <c r="J35" s="49" t="str">
         <f t="array" ref="J35">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="39" t="str">
+      <c r="B36" s="44" t="str">
         <f t="array" ref="B36">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="C36" s="19" t="str">
+      <c r="C36" s="45" t="str">
         <f t="array" ref="C36">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="D36" s="39" t="str">
+      <c r="D36" s="46" t="str">
         <f t="array" ref="D36">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="E36" s="39" t="str">
+      <c r="E36" s="46" t="str">
         <f t="array" ref="E36">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="F36" s="40" t="str">
+      <c r="F36" s="47" t="str">
         <f t="array" ref="F36">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="G36" s="39" t="str">
+      <c r="G36" s="46" t="str">
         <f t="array" ref="G36">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="H36" s="33" t="str">
+      <c r="H36" s="46" t="str">
         <f t="array" ref="H36">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="I36" s="39" t="str">
+      <c r="I36" s="48" t="str">
         <f t="array" ref="I36">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="J36" s="19" t="str">
+      <c r="J36" s="49" t="str">
         <f t="array" ref="J36">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="39" t="str">
+      <c r="B37" s="44" t="str">
         <f t="array" ref="B37">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="C37" s="19" t="str">
+      <c r="C37" s="45" t="str">
         <f t="array" ref="C37">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="D37" s="39" t="str">
+      <c r="D37" s="46" t="str">
         <f t="array" ref="D37">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="E37" s="39" t="str">
+      <c r="E37" s="46" t="str">
         <f t="array" ref="E37">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="F37" s="40" t="str">
+      <c r="F37" s="47" t="str">
         <f t="array" ref="F37">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="G37" s="39" t="str">
+      <c r="G37" s="46" t="str">
         <f t="array" ref="G37">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="H37" s="33" t="str">
+      <c r="H37" s="46" t="str">
         <f t="array" ref="H37">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="I37" s="39" t="str">
+      <c r="I37" s="48" t="str">
         <f t="array" ref="I37">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="J37" s="19" t="str">
+      <c r="J37" s="49" t="str">
         <f t="array" ref="J37">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="str">
+      <c r="B38" s="44" t="str">
         <f t="array" ref="B38">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="C38" s="19" t="str">
+      <c r="C38" s="45" t="str">
         <f t="array" ref="C38">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="D38" s="39" t="str">
+      <c r="D38" s="46" t="str">
         <f t="array" ref="D38">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="E38" s="39" t="str">
+      <c r="E38" s="46" t="str">
         <f t="array" ref="E38">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="F38" s="40" t="str">
+      <c r="F38" s="47" t="str">
         <f t="array" ref="F38">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="G38" s="39" t="str">
+      <c r="G38" s="46" t="str">
         <f t="array" ref="G38">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="H38" s="33" t="str">
+      <c r="H38" s="46" t="str">
         <f t="array" ref="H38">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="I38" s="39" t="str">
+      <c r="I38" s="48" t="str">
         <f t="array" ref="I38">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="J38" s="19" t="str">
+      <c r="J38" s="49" t="str">
         <f t="array" ref="J38">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="str">
+      <c r="B39" s="44" t="str">
         <f t="array" ref="B39">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="C39" s="19" t="str">
+      <c r="C39" s="45" t="str">
         <f t="array" ref="C39">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="D39" s="39" t="str">
+      <c r="D39" s="46" t="str">
         <f t="array" ref="D39">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="E39" s="39" t="str">
+      <c r="E39" s="46" t="str">
         <f t="array" ref="E39">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="F39" s="40" t="str">
+      <c r="F39" s="47" t="str">
         <f t="array" ref="F39">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="G39" s="39" t="str">
+      <c r="G39" s="46" t="str">
         <f t="array" ref="G39">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="H39" s="33" t="str">
+      <c r="H39" s="46" t="str">
         <f t="array" ref="H39">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="I39" s="39" t="str">
+      <c r="I39" s="48" t="str">
         <f t="array" ref="I39">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="J39" s="19" t="str">
+      <c r="J39" s="49" t="str">
         <f t="array" ref="J39">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="39" t="str">
+      <c r="B40" s="44" t="str">
         <f t="array" ref="B40">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="C40" s="19" t="str">
+      <c r="C40" s="45" t="str">
         <f t="array" ref="C40">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="D40" s="39" t="str">
+      <c r="D40" s="46" t="str">
         <f t="array" ref="D40">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="E40" s="39" t="str">
+      <c r="E40" s="46" t="str">
         <f t="array" ref="E40">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="F40" s="40" t="str">
+      <c r="F40" s="47" t="str">
         <f t="array" ref="F40">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="G40" s="39" t="str">
+      <c r="G40" s="46" t="str">
         <f t="array" ref="G40">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="H40" s="33" t="str">
+      <c r="H40" s="46" t="str">
         <f t="array" ref="H40">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="I40" s="39" t="str">
+      <c r="I40" s="48" t="str">
         <f t="array" ref="I40">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="J40" s="19" t="str">
+      <c r="J40" s="49" t="str">
         <f t="array" ref="J40">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="39" t="str">
+      <c r="B41" s="44" t="str">
         <f t="array" ref="B41">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="C41" s="19" t="str">
+      <c r="C41" s="45" t="str">
         <f t="array" ref="C41">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="D41" s="39" t="str">
+      <c r="D41" s="46" t="str">
         <f t="array" ref="D41">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="E41" s="39" t="str">
+      <c r="E41" s="46" t="str">
         <f t="array" ref="E41">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="F41" s="40" t="str">
+      <c r="F41" s="47" t="str">
         <f t="array" ref="F41">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="G41" s="39" t="str">
+      <c r="G41" s="46" t="str">
         <f t="array" ref="G41">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="H41" s="33" t="str">
+      <c r="H41" s="46" t="str">
         <f t="array" ref="H41">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="I41" s="39" t="str">
+      <c r="I41" s="48" t="str">
         <f t="array" ref="I41">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="J41" s="19" t="str">
+      <c r="J41" s="49" t="str">
         <f t="array" ref="J41">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="39" t="str">
+      <c r="B42" s="44" t="str">
         <f t="array" ref="B42">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="C42" s="19" t="str">
+      <c r="C42" s="45" t="str">
         <f t="array" ref="C42">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="D42" s="39" t="str">
+      <c r="D42" s="46" t="str">
         <f t="array" ref="D42">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="E42" s="39" t="str">
+      <c r="E42" s="46" t="str">
         <f t="array" ref="E42">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="F42" s="40" t="str">
+      <c r="F42" s="47" t="str">
         <f t="array" ref="F42">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="G42" s="39" t="str">
+      <c r="G42" s="46" t="str">
         <f t="array" ref="G42">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="H42" s="33" t="str">
+      <c r="H42" s="46" t="str">
         <f t="array" ref="H42">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="I42" s="39" t="str">
+      <c r="I42" s="48" t="str">
         <f t="array" ref="I42">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="J42" s="19" t="str">
+      <c r="J42" s="49" t="str">
         <f t="array" ref="J42">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="39" t="str">
+      <c r="B43" s="44" t="str">
         <f t="array" ref="B43">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="C43" s="19" t="str">
+      <c r="C43" s="45" t="str">
         <f t="array" ref="C43">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="D43" s="39" t="str">
+      <c r="D43" s="46" t="str">
         <f t="array" ref="D43">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="E43" s="39" t="str">
+      <c r="E43" s="46" t="str">
         <f t="array" ref="E43">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="F43" s="40" t="str">
+      <c r="F43" s="47" t="str">
         <f t="array" ref="F43">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="G43" s="39" t="str">
+      <c r="G43" s="46" t="str">
         <f t="array" ref="G43">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="H43" s="33" t="str">
+      <c r="H43" s="46" t="str">
         <f t="array" ref="H43">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="I43" s="39" t="str">
+      <c r="I43" s="48" t="str">
         <f t="array" ref="I43">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="J43" s="19" t="str">
+      <c r="J43" s="49" t="str">
         <f t="array" ref="J43">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="39" t="str">
+      <c r="B44" s="44" t="str">
         <f t="array" ref="B44">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="C44" s="19" t="str">
+      <c r="C44" s="45" t="str">
         <f t="array" ref="C44">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="D44" s="39" t="str">
+      <c r="D44" s="46" t="str">
         <f t="array" ref="D44">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="E44" s="39" t="str">
+      <c r="E44" s="46" t="str">
         <f t="array" ref="E44">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="F44" s="40" t="str">
+      <c r="F44" s="47" t="str">
         <f t="array" ref="F44">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="G44" s="39" t="str">
+      <c r="G44" s="46" t="str">
         <f t="array" ref="G44">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="H44" s="33" t="str">
+      <c r="H44" s="46" t="str">
         <f t="array" ref="H44">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="I44" s="39" t="str">
+      <c r="I44" s="48" t="str">
         <f t="array" ref="I44">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="J44" s="19" t="str">
+      <c r="J44" s="49" t="str">
         <f t="array" ref="J44">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="39" t="str">
+      <c r="B45" s="44" t="str">
         <f t="array" ref="B45">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="C45" s="19" t="str">
+      <c r="C45" s="45" t="str">
         <f t="array" ref="C45">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="D45" s="39" t="str">
+      <c r="D45" s="46" t="str">
         <f t="array" ref="D45">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="E45" s="39" t="str">
+      <c r="E45" s="46" t="str">
         <f t="array" ref="E45">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="F45" s="40" t="str">
+      <c r="F45" s="47" t="str">
         <f t="array" ref="F45">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="G45" s="39" t="str">
+      <c r="G45" s="46" t="str">
         <f t="array" ref="G45">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="H45" s="33" t="str">
+      <c r="H45" s="46" t="str">
         <f t="array" ref="H45">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="I45" s="39" t="str">
+      <c r="I45" s="48" t="str">
         <f t="array" ref="I45">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="J45" s="19" t="str">
+      <c r="J45" s="49" t="str">
         <f t="array" ref="J45">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="39" t="str">
+      <c r="B46" s="44" t="str">
         <f t="array" ref="B46">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="C46" s="19" t="str">
+      <c r="C46" s="45" t="str">
         <f t="array" ref="C46">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="D46" s="39" t="str">
+      <c r="D46" s="46" t="str">
         <f t="array" ref="D46">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="E46" s="39" t="str">
+      <c r="E46" s="46" t="str">
         <f t="array" ref="E46">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="F46" s="40" t="str">
+      <c r="F46" s="47" t="str">
         <f t="array" ref="F46">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="G46" s="39" t="str">
+      <c r="G46" s="46" t="str">
         <f t="array" ref="G46">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="H46" s="33" t="str">
+      <c r="H46" s="46" t="str">
         <f t="array" ref="H46">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="I46" s="39" t="str">
+      <c r="I46" s="48" t="str">
         <f t="array" ref="I46">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="J46" s="19" t="str">
+      <c r="J46" s="49" t="str">
         <f t="array" ref="J46">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="39" t="str">
+      <c r="B47" s="44" t="str">
         <f t="array" ref="B47">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="C47" s="19" t="str">
+      <c r="C47" s="45" t="str">
         <f t="array" ref="C47">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="D47" s="39" t="str">
+      <c r="D47" s="46" t="str">
         <f t="array" ref="D47">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="E47" s="39" t="str">
+      <c r="E47" s="46" t="str">
         <f t="array" ref="E47">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="F47" s="40" t="str">
+      <c r="F47" s="47" t="str">
         <f t="array" ref="F47">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="G47" s="39" t="str">
+      <c r="G47" s="46" t="str">
         <f t="array" ref="G47">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="H47" s="33" t="str">
+      <c r="H47" s="46" t="str">
         <f t="array" ref="H47">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="I47" s="39" t="str">
+      <c r="I47" s="48" t="str">
         <f t="array" ref="I47">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="J47" s="19" t="str">
+      <c r="J47" s="49" t="str">
         <f t="array" ref="J47">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="39" t="str">
+      <c r="B48" s="44" t="str">
         <f t="array" ref="B48">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="C48" s="19" t="str">
+      <c r="C48" s="45" t="str">
         <f t="array" ref="C48">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="D48" s="39" t="str">
+      <c r="D48" s="46" t="str">
         <f t="array" ref="D48">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="E48" s="39" t="str">
+      <c r="E48" s="46" t="str">
         <f t="array" ref="E48">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="F48" s="40" t="str">
+      <c r="F48" s="47" t="str">
         <f t="array" ref="F48">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="G48" s="39" t="str">
+      <c r="G48" s="46" t="str">
         <f t="array" ref="G48">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="H48" s="33" t="str">
+      <c r="H48" s="46" t="str">
         <f t="array" ref="H48">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="I48" s="39" t="str">
+      <c r="I48" s="48" t="str">
         <f t="array" ref="I48">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="J48" s="19" t="str">
+      <c r="J48" s="49" t="str">
         <f t="array" ref="J48">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="39" t="str">
+      <c r="B49" s="44" t="str">
         <f t="array" ref="B49">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="C49" s="19" t="str">
+      <c r="C49" s="45" t="str">
         <f t="array" ref="C49">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="D49" s="39" t="str">
+      <c r="D49" s="46" t="str">
         <f t="array" ref="D49">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="E49" s="39" t="str">
+      <c r="E49" s="46" t="str">
         <f t="array" ref="E49">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="F49" s="40" t="str">
+      <c r="F49" s="47" t="str">
         <f t="array" ref="F49">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="G49" s="39" t="str">
+      <c r="G49" s="46" t="str">
         <f t="array" ref="G49">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="H49" s="33" t="str">
+      <c r="H49" s="46" t="str">
         <f t="array" ref="H49">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="I49" s="39" t="str">
+      <c r="I49" s="48" t="str">
         <f t="array" ref="I49">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="J49" s="19" t="str">
+      <c r="J49" s="49" t="str">
         <f t="array" ref="J49">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="39" t="str">
+      <c r="B50" s="44" t="str">
         <f t="array" ref="B50">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="C50" s="19" t="str">
+      <c r="C50" s="45" t="str">
         <f t="array" ref="C50">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="D50" s="39" t="str">
+      <c r="D50" s="46" t="str">
         <f t="array" ref="D50">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="E50" s="39" t="str">
+      <c r="E50" s="46" t="str">
         <f t="array" ref="E50">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="F50" s="40" t="str">
+      <c r="F50" s="47" t="str">
         <f t="array" ref="F50">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="G50" s="39" t="str">
+      <c r="G50" s="46" t="str">
         <f t="array" ref="G50">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="H50" s="33" t="str">
+      <c r="H50" s="46" t="str">
         <f t="array" ref="H50">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="I50" s="39" t="str">
+      <c r="I50" s="48" t="str">
         <f t="array" ref="I50">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="J50" s="19" t="str">
+      <c r="J50" s="49" t="str">
         <f t="array" ref="J50">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="39" t="str">
+      <c r="B51" s="44" t="str">
         <f t="array" ref="B51">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="C51" s="19" t="str">
+      <c r="C51" s="45" t="str">
         <f t="array" ref="C51">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="D51" s="39" t="str">
+      <c r="D51" s="46" t="str">
         <f t="array" ref="D51">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="E51" s="39" t="str">
+      <c r="E51" s="46" t="str">
         <f t="array" ref="E51">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="F51" s="40" t="str">
+      <c r="F51" s="47" t="str">
         <f t="array" ref="F51">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="G51" s="39" t="str">
+      <c r="G51" s="46" t="str">
         <f t="array" ref="G51">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="H51" s="33" t="str">
+      <c r="H51" s="46" t="str">
         <f t="array" ref="H51">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="I51" s="39" t="str">
+      <c r="I51" s="48" t="str">
         <f t="array" ref="I51">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="J51" s="19" t="str">
+      <c r="J51" s="49" t="str">
         <f t="array" ref="J51">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="39" t="str">
+      <c r="B52" s="44" t="str">
         <f t="array" ref="B52">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="C52" s="19" t="str">
+      <c r="C52" s="45" t="str">
         <f t="array" ref="C52">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="D52" s="39" t="str">
+      <c r="D52" s="46" t="str">
         <f t="array" ref="D52">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="E52" s="39" t="str">
+      <c r="E52" s="46" t="str">
         <f t="array" ref="E52">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="F52" s="40" t="str">
+      <c r="F52" s="47" t="str">
         <f t="array" ref="F52">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="G52" s="39" t="str">
+      <c r="G52" s="46" t="str">
         <f t="array" ref="G52">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="H52" s="33" t="str">
+      <c r="H52" s="46" t="str">
         <f t="array" ref="H52">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="I52" s="39" t="str">
+      <c r="I52" s="48" t="str">
         <f t="array" ref="I52">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="J52" s="19" t="str">
+      <c r="J52" s="49" t="str">
         <f t="array" ref="J52">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="39" t="str">
+      <c r="B53" s="44" t="str">
         <f t="array" ref="B53">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="C53" s="19" t="str">
+      <c r="C53" s="45" t="str">
         <f t="array" ref="C53">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="D53" s="39" t="str">
+      <c r="D53" s="46" t="str">
         <f t="array" ref="D53">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="E53" s="39" t="str">
+      <c r="E53" s="46" t="str">
         <f t="array" ref="E53">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="F53" s="40" t="str">
+      <c r="F53" s="47" t="str">
         <f t="array" ref="F53">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="G53" s="39" t="str">
+      <c r="G53" s="46" t="str">
         <f t="array" ref="G53">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="H53" s="33" t="str">
+      <c r="H53" s="46" t="str">
         <f t="array" ref="H53">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="I53" s="39" t="str">
+      <c r="I53" s="48" t="str">
         <f t="array" ref="I53">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="J53" s="19" t="str">
+      <c r="J53" s="49" t="str">
         <f t="array" ref="J53">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="39" t="str">
+      <c r="B54" s="44" t="str">
         <f t="array" ref="B54">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="C54" s="19" t="str">
+      <c r="C54" s="45" t="str">
         <f t="array" ref="C54">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="D54" s="39" t="str">
+      <c r="D54" s="46" t="str">
         <f t="array" ref="D54">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="E54" s="39" t="str">
+      <c r="E54" s="46" t="str">
         <f t="array" ref="E54">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="F54" s="40" t="str">
+      <c r="F54" s="47" t="str">
         <f t="array" ref="F54">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="G54" s="39" t="str">
+      <c r="G54" s="46" t="str">
         <f t="array" ref="G54">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="H54" s="33" t="str">
+      <c r="H54" s="46" t="str">
         <f t="array" ref="H54">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="I54" s="39" t="str">
+      <c r="I54" s="48" t="str">
         <f t="array" ref="I54">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="J54" s="19" t="str">
+      <c r="J54" s="49" t="str">
         <f t="array" ref="J54">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="20" t="str">
+      <c r="B55" s="50" t="str">
         <f t="array" ref="B55">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="C55" s="21" t="str">
+      <c r="C55" s="51" t="str">
         <f t="array" ref="C55">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="D55" s="20" t="str">
+      <c r="D55" s="52" t="str">
         <f t="array" ref="D55">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="E55" s="20" t="str">
+      <c r="E55" s="52" t="str">
         <f t="array" ref="E55">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="F55" s="22" t="str">
+      <c r="F55" s="53" t="str">
         <f t="array" ref="F55">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="G55" s="20" t="str">
+      <c r="G55" s="52" t="str">
         <f t="array" ref="G55">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="H55" s="34" t="str">
+      <c r="H55" s="52" t="str">
         <f t="array" ref="H55">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="I55" s="20" t="str">
+      <c r="I55" s="54" t="str">
         <f t="array" ref="I55">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="J55" s="21" t="str">
+      <c r="J55" s="55" t="str">
         <f t="array" ref="J55">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rHWjBQR5Qqic9iItYVKaQP4eg7hzOXsWAsZiPyKZF0omAXyW/Rxf2qICdVJmT7R18/K7tUtdff9QbmcJkCoCtg==" saltValue="EkExKNYtiZ3w5hp17N3KlA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
@@ -5209,21 +5124,18 @@
     <mergeCell ref="M16:M17"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
       <formula>$H$4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -5231,9 +5143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262A3E2A-86CA-4231-B82B-405B67DE33BC}">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5292,6 +5204,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" s="3"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
@@ -5767,42 +5680,58 @@
       <c r="E161" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C161">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="C1 C17:C161">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C161">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+  <conditionalFormatting sqref="C17:C161">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"PAGO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C16">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"INVESTIMENTO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C16">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"PARCELADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"PENDENTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C162:C1048576" xr:uid="{8F5598F2-1887-4907-A141-5ACA1B7011F5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C162:C1048576 C2:C16" xr:uid="{8F5598F2-1887-4907-A141-5ACA1B7011F5}">
       <formula1>"PAGO,PENDENTE,PARCELADO,INVESTIMENTO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C161" xr:uid="{2922D9E2-37F4-49CA-A6CF-FFA4850A6792}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C161" xr:uid="{2922D9E2-37F4-49CA-A6CF-FFA4850A6792}">
       <formula1>"PAGO,PENDENTE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5818,7 +5747,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D7"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Nova atualização da planilha financeira
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7635C129-411D-4C17-8CE9-2FE31DAD5AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746B6A63-6C48-4A38-A99E-5721A0AF01F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
@@ -617,6 +617,72 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,138 +701,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -869,6 +809,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2757,31 +2701,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}" name="R_TABELA" displayName="R_TABELA" ref="A1:I161" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
   <autoFilter ref="A1:I161" xr:uid="{2B2CDC24-5381-4190-B0AA-512CE559C836}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{470E75A0-F5FC-4E6E-8D5E-C9BDCC219D2D}" name="DESCRIÇÃO" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="4" totalsRowDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{137BCC31-E147-443F-B9DD-EAE3E800C93E}" name="VALOR" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{A37D1309-20C9-4AEF-85AE-1F8A5C50FFD2}" name="STATUS" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{3F01F472-429E-4F5B-9227-5FC52DA83C1C}" name="CATEGORIA" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0FDE0BD6-B7BF-47D3-BA36-167638AA766D}" name="DATA DE VENCIMENTO" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{64B2A404-82F0-4BC1-ABD5-2F868A21F88A}" name="FORMA DE PAGAMENTO" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{77BBC10F-1D7A-40E5-9492-EAC8CBDCAF50}" name="PARCELA" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{768056F7-CE80-4A44-9E85-3F6DE22F4D68}" name="MÊS/ANO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{BD1933C7-91CB-49AD-BC18-7DD065229BCF}" name="OBSERVAÇÕES" totalsRowFunction="count" dataDxfId="18" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}" name="R_ENTRADA" displayName="R_ENTRADA" ref="A1:D8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:D8" xr:uid="{9D6A42F9-419D-4A14-AE17-402838E2E5E9}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="20" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{BE7DB68E-BA79-4FFD-B30A-9EF66D17D86C}" name="MÊS" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DE44CCC1-3962-46CC-A574-121D3488A812}" name="ANO" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{CDD0DBB4-2F42-41F2-9675-F11B64626ED8}" name="DESCRIÇÃO" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{28C765A0-2054-4B9C-BE18-5214088D2687}" name="VALOR" dataDxfId="11" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3087,7 +3031,7 @@
   <dimension ref="B1:M56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,11 +3062,11 @@
       <c r="C2" s="24">
         <v>8</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="L2" s="17" t="s">
         <v>9</v>
       </c>
@@ -3138,9 +3082,9 @@
       <c r="C3" s="24">
         <v>2025</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
       <c r="I3" s="22" t="s">
         <v>14</v>
       </c>
@@ -3159,12 +3103,12 @@
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19"/>
       <c r="C4" s="25"/>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="27">
         <f>SUM(C6:C55)</f>
         <v>0</v>
@@ -3178,1945 +3122,1946 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="str">
+      <c r="B6" s="32" t="str">
         <f t="array" ref="B6">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="C6" s="39" t="str">
+      <c r="C6" s="33" t="str">
         <f t="array" ref="C6">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="D6" s="40" t="str">
+      <c r="D6" s="34" t="str">
         <f t="array" ref="D6">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="E6" s="40" t="str">
+      <c r="E6" s="34" t="str">
         <f t="array" ref="E6">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="F6" s="41" t="str">
+      <c r="F6" s="35" t="str">
         <f t="array" ref="F6">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="G6" s="40" t="str">
+      <c r="G6" s="34" t="str">
         <f t="array" ref="G6">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="H6" s="40" t="str">
+      <c r="H6" s="34" t="str">
         <f t="array" ref="H6">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="I6" s="42" t="str">
+      <c r="I6" s="36" t="str">
         <f t="array" ref="I6">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
-      <c r="J6" s="43" t="str">
+      <c r="J6" s="37" t="str">
         <f t="array" ref="J6">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(1:1))),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="str">
+      <c r="B7" s="38" t="str">
         <f t="array" ref="B7">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="C7" s="45" t="str">
+      <c r="C7" s="39" t="str">
         <f t="array" ref="C7">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="D7" s="46" t="str">
+      <c r="D7" s="40" t="str">
         <f t="array" ref="D7">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="E7" s="46" t="str">
+      <c r="E7" s="40" t="str">
         <f t="array" ref="E7">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="F7" s="47" t="str">
+      <c r="F7" s="41" t="str">
         <f t="array" ref="F7">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="G7" s="46" t="str">
+      <c r="G7" s="40" t="str">
         <f t="array" ref="G7">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="H7" s="46" t="str">
+      <c r="H7" s="40" t="str">
         <f t="array" ref="H7">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="I7" s="48" t="str">
+      <c r="I7" s="42" t="str">
         <f t="array" ref="I7">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
-      <c r="J7" s="49" t="str">
+      <c r="J7" s="43" t="str">
         <f t="array" ref="J7">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(2:2))),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="str">
+      <c r="B8" s="38" t="str">
         <f t="array" ref="B8">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="C8" s="45" t="str">
+      <c r="C8" s="39" t="str">
         <f t="array" ref="C8">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="D8" s="46" t="str">
+      <c r="D8" s="40" t="str">
         <f t="array" ref="D8">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="E8" s="46" t="str">
+      <c r="E8" s="40" t="str">
         <f t="array" ref="E8">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="F8" s="47" t="str">
+      <c r="F8" s="41" t="str">
         <f t="array" ref="F8">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="G8" s="46" t="str">
+      <c r="G8" s="40" t="str">
         <f t="array" ref="G8">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="H8" s="46" t="str">
+      <c r="H8" s="40" t="str">
         <f t="array" ref="H8">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="I8" s="48" t="str">
+      <c r="I8" s="42" t="str">
         <f t="array" ref="I8">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
-      <c r="J8" s="49" t="str">
+      <c r="J8" s="43" t="str">
         <f t="array" ref="J8">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(3:3))),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="str">
+      <c r="B9" s="38" t="str">
         <f t="array" ref="B9">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="C9" s="45" t="str">
+      <c r="C9" s="39" t="str">
         <f t="array" ref="C9">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="D9" s="46" t="str">
+      <c r="D9" s="40" t="str">
         <f t="array" ref="D9">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="E9" s="46" t="str">
+      <c r="E9" s="40" t="str">
         <f t="array" ref="E9">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="F9" s="47" t="str">
+      <c r="F9" s="41" t="str">
         <f t="array" ref="F9">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="G9" s="46" t="str">
+      <c r="G9" s="40" t="str">
         <f t="array" ref="G9">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="H9" s="46" t="str">
+      <c r="H9" s="40" t="str">
         <f t="array" ref="H9">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="I9" s="48" t="str">
+      <c r="I9" s="42" t="str">
         <f t="array" ref="I9">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
-      <c r="J9" s="49" t="str">
+      <c r="J9" s="43" t="str">
         <f t="array" ref="J9">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(4:4))),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="str">
+      <c r="B10" s="38" t="str">
         <f t="array" ref="B10">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="C10" s="45" t="str">
+      <c r="C10" s="39" t="str">
         <f t="array" ref="C10">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="D10" s="46" t="str">
+      <c r="D10" s="40" t="str">
         <f t="array" ref="D10">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="E10" s="46" t="str">
+      <c r="E10" s="40" t="str">
         <f t="array" ref="E10">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="F10" s="47" t="str">
+      <c r="F10" s="41" t="str">
         <f t="array" ref="F10">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="G10" s="46" t="str">
+      <c r="G10" s="40" t="str">
         <f t="array" ref="G10">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="H10" s="46" t="str">
+      <c r="H10" s="40" t="str">
         <f t="array" ref="H10">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="I10" s="48" t="str">
+      <c r="I10" s="42" t="str">
         <f t="array" ref="I10">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
-      <c r="J10" s="49" t="str">
+      <c r="J10" s="43" t="str">
         <f t="array" ref="J10">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(5:5))),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="str">
+      <c r="B11" s="38" t="str">
         <f t="array" ref="B11">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="C11" s="45" t="str">
+      <c r="C11" s="39" t="str">
         <f t="array" ref="C11">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="D11" s="46" t="str">
+      <c r="D11" s="40" t="str">
         <f t="array" ref="D11">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="E11" s="46" t="str">
+      <c r="E11" s="40" t="str">
         <f t="array" ref="E11">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="F11" s="47" t="str">
+      <c r="F11" s="41" t="str">
         <f t="array" ref="F11">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="G11" s="46" t="str">
+      <c r="G11" s="40" t="str">
         <f t="array" ref="G11">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="H11" s="46" t="str">
+      <c r="H11" s="40" t="str">
         <f t="array" ref="H11">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="I11" s="48" t="str">
+      <c r="I11" s="42" t="str">
         <f t="array" ref="I11">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
-      <c r="J11" s="49" t="str">
+      <c r="J11" s="43" t="str">
         <f t="array" ref="J11">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(6:6))),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="str">
+      <c r="B12" s="38" t="str">
         <f t="array" ref="B12">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="C12" s="45" t="str">
+      <c r="C12" s="39" t="str">
         <f t="array" ref="C12">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="D12" s="46" t="str">
+      <c r="D12" s="40" t="str">
         <f t="array" ref="D12">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="E12" s="46" t="str">
+      <c r="E12" s="40" t="str">
         <f t="array" ref="E12">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="F12" s="47" t="str">
+      <c r="F12" s="41" t="str">
         <f t="array" ref="F12">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="G12" s="46" t="str">
+      <c r="G12" s="40" t="str">
         <f t="array" ref="G12">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="H12" s="46" t="str">
+      <c r="H12" s="40" t="str">
         <f t="array" ref="H12">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="I12" s="48" t="str">
+      <c r="I12" s="42" t="str">
         <f t="array" ref="I12">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
-      <c r="J12" s="49" t="str">
+      <c r="J12" s="43" t="str">
         <f t="array" ref="J12">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(7:7))),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="str">
+      <c r="B13" s="38" t="str">
         <f t="array" ref="B13">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="C13" s="45" t="str">
+      <c r="C13" s="39" t="str">
         <f t="array" ref="C13">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="D13" s="46" t="str">
+      <c r="D13" s="40" t="str">
         <f t="array" ref="D13">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="E13" s="46" t="str">
+      <c r="E13" s="40" t="str">
         <f t="array" ref="E13">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="F13" s="47" t="str">
+      <c r="F13" s="41" t="str">
         <f t="array" ref="F13">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="G13" s="46" t="str">
+      <c r="G13" s="40" t="str">
         <f t="array" ref="G13">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="H13" s="46" t="str">
+      <c r="H13" s="40" t="str">
         <f t="array" ref="H13">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="I13" s="48" t="str">
+      <c r="I13" s="42" t="str">
         <f t="array" ref="I13">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
-      <c r="J13" s="49" t="str">
+      <c r="J13" s="43" t="str">
         <f t="array" ref="J13">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(8:8))),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="str">
+      <c r="B14" s="38" t="str">
         <f t="array" ref="B14">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="C14" s="45" t="str">
+      <c r="C14" s="39" t="str">
         <f t="array" ref="C14">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="D14" s="46" t="str">
+      <c r="D14" s="40" t="str">
         <f t="array" ref="D14">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="E14" s="46" t="str">
+      <c r="E14" s="40" t="str">
         <f t="array" ref="E14">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="F14" s="47" t="str">
+      <c r="F14" s="41" t="str">
         <f t="array" ref="F14">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="G14" s="46" t="str">
+      <c r="G14" s="40" t="str">
         <f t="array" ref="G14">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="H14" s="46" t="str">
+      <c r="H14" s="40" t="str">
         <f t="array" ref="H14">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="I14" s="48" t="str">
+      <c r="I14" s="42" t="str">
         <f t="array" ref="I14">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
-      <c r="J14" s="49" t="str">
+      <c r="J14" s="43" t="str">
         <f t="array" ref="J14">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(9:9))),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="44" t="str">
+      <c r="B15" s="38" t="str">
         <f t="array" ref="B15">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="C15" s="45" t="str">
+      <c r="C15" s="39" t="str">
         <f t="array" ref="C15">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="D15" s="46" t="str">
+      <c r="D15" s="40" t="str">
         <f t="array" ref="D15">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="E15" s="46" t="str">
+      <c r="E15" s="40" t="str">
         <f t="array" ref="E15">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="F15" s="47" t="str">
+      <c r="F15" s="41" t="str">
         <f t="array" ref="F15">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="G15" s="46" t="str">
+      <c r="G15" s="40" t="str">
         <f t="array" ref="G15">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="H15" s="46" t="str">
+      <c r="H15" s="40" t="str">
         <f t="array" ref="H15">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="I15" s="48" t="str">
+      <c r="I15" s="42" t="str">
         <f t="array" ref="I15">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
-      <c r="J15" s="49" t="str">
+      <c r="J15" s="43" t="str">
         <f t="array" ref="J15">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(10:10))),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="str">
+      <c r="B16" s="38" t="str">
         <f t="array" ref="B16">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="C16" s="45" t="str">
+      <c r="C16" s="39" t="str">
         <f t="array" ref="C16">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="D16" s="46" t="str">
+      <c r="D16" s="40" t="str">
         <f t="array" ref="D16">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="E16" s="46" t="str">
+      <c r="E16" s="40" t="str">
         <f t="array" ref="E16">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="F16" s="47" t="str">
+      <c r="F16" s="41" t="str">
         <f t="array" ref="F16">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="G16" s="46" t="str">
+      <c r="G16" s="40" t="str">
         <f t="array" ref="G16">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="H16" s="46" t="str">
+      <c r="H16" s="40" t="str">
         <f t="array" ref="H16">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="I16" s="48" t="str">
+      <c r="I16" s="42" t="str">
         <f t="array" ref="I16">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="J16" s="49" t="str">
+      <c r="J16" s="43" t="str">
         <f t="array" ref="J16">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(11:11))),"")</f>
         <v/>
       </c>
-      <c r="L16" s="30" t="s">
+      <c r="L16" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16" s="54">
         <f>J4-H4</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="44" t="str">
+      <c r="B17" s="38" t="str">
         <f t="array" ref="B17">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="C17" s="45" t="str">
+      <c r="C17" s="39" t="str">
         <f t="array" ref="C17">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="D17" s="46" t="str">
+      <c r="D17" s="40" t="str">
         <f t="array" ref="D17">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="E17" s="46" t="str">
+      <c r="E17" s="40" t="str">
         <f t="array" ref="E17">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="F17" s="47" t="str">
+      <c r="F17" s="41" t="str">
         <f t="array" ref="F17">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="G17" s="46" t="str">
+      <c r="G17" s="40" t="str">
         <f t="array" ref="G17">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="H17" s="46" t="str">
+      <c r="H17" s="40" t="str">
         <f t="array" ref="H17">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="I17" s="48" t="str">
+      <c r="I17" s="42" t="str">
         <f t="array" ref="I17">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="J17" s="49" t="str">
+      <c r="J17" s="43" t="str">
         <f t="array" ref="J17">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(12:12))),"")</f>
         <v/>
       </c>
-      <c r="L17" s="31"/>
-      <c r="M17" s="33"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="55"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="str">
+      <c r="B18" s="38" t="str">
         <f t="array" ref="B18">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="C18" s="45" t="str">
+      <c r="C18" s="39" t="str">
         <f t="array" ref="C18">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="D18" s="46" t="str">
+      <c r="D18" s="40" t="str">
         <f t="array" ref="D18">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="E18" s="46" t="str">
+      <c r="E18" s="40" t="str">
         <f t="array" ref="E18">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="F18" s="47" t="str">
+      <c r="F18" s="41" t="str">
         <f t="array" ref="F18">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="G18" s="46" t="str">
+      <c r="G18" s="40" t="str">
         <f t="array" ref="G18">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="H18" s="46" t="str">
+      <c r="H18" s="40" t="str">
         <f t="array" ref="H18">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="I18" s="48" t="str">
+      <c r="I18" s="42" t="str">
         <f t="array" ref="I18">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
-      <c r="J18" s="49" t="str">
+      <c r="J18" s="43" t="str">
         <f t="array" ref="J18">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(13:13))),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="str">
+      <c r="B19" s="38" t="str">
         <f t="array" ref="B19">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="C19" s="45" t="str">
+      <c r="C19" s="39" t="str">
         <f t="array" ref="C19">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="D19" s="46" t="str">
+      <c r="D19" s="40" t="str">
         <f t="array" ref="D19">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="E19" s="46" t="str">
+      <c r="E19" s="40" t="str">
         <f t="array" ref="E19">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="F19" s="47" t="str">
+      <c r="F19" s="41" t="str">
         <f t="array" ref="F19">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="G19" s="46" t="str">
+      <c r="G19" s="40" t="str">
         <f t="array" ref="G19">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="H19" s="46" t="str">
+      <c r="H19" s="40" t="str">
         <f t="array" ref="H19">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="I19" s="48" t="str">
+      <c r="I19" s="42" t="str">
         <f t="array" ref="I19">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
-      <c r="J19" s="49" t="str">
+      <c r="J19" s="43" t="str">
         <f t="array" ref="J19">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(14:14))),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="str">
+      <c r="B20" s="38" t="str">
         <f t="array" ref="B20">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="C20" s="45" t="str">
+      <c r="C20" s="39" t="str">
         <f t="array" ref="C20">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="D20" s="46" t="str">
+      <c r="D20" s="40" t="str">
         <f t="array" ref="D20">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="E20" s="46" t="str">
+      <c r="E20" s="40" t="str">
         <f t="array" ref="E20">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="F20" s="47" t="str">
+      <c r="F20" s="41" t="str">
         <f t="array" ref="F20">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="G20" s="46" t="str">
+      <c r="G20" s="40" t="str">
         <f t="array" ref="G20">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="H20" s="46" t="str">
+      <c r="H20" s="40" t="str">
         <f t="array" ref="H20">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="I20" s="48" t="str">
+      <c r="I20" s="42" t="str">
         <f t="array" ref="I20">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
-      <c r="J20" s="49" t="str">
+      <c r="J20" s="43" t="str">
         <f t="array" ref="J20">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(15:15))),"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="str">
+      <c r="B21" s="38" t="str">
         <f t="array" ref="B21">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="C21" s="45" t="str">
+      <c r="C21" s="39" t="str">
         <f t="array" ref="C21">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="D21" s="46" t="str">
+      <c r="D21" s="40" t="str">
         <f t="array" ref="D21">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="E21" s="46" t="str">
+      <c r="E21" s="40" t="str">
         <f t="array" ref="E21">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="F21" s="47" t="str">
+      <c r="F21" s="41" t="str">
         <f t="array" ref="F21">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="G21" s="46" t="str">
+      <c r="G21" s="40" t="str">
         <f t="array" ref="G21">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="H21" s="46" t="str">
+      <c r="H21" s="40" t="str">
         <f t="array" ref="H21">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="I21" s="48" t="str">
+      <c r="I21" s="42" t="str">
         <f t="array" ref="I21">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
-      <c r="J21" s="49" t="str">
+      <c r="J21" s="43" t="str">
         <f t="array" ref="J21">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(16:16))),"")</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="str">
+      <c r="B22" s="38" t="str">
         <f t="array" ref="B22">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="C22" s="45" t="str">
+      <c r="C22" s="39" t="str">
         <f t="array" ref="C22">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="D22" s="46" t="str">
+      <c r="D22" s="40" t="str">
         <f t="array" ref="D22">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="E22" s="46" t="str">
+      <c r="E22" s="40" t="str">
         <f t="array" ref="E22">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="F22" s="47" t="str">
+      <c r="F22" s="41" t="str">
         <f t="array" ref="F22">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="G22" s="46" t="str">
+      <c r="G22" s="40" t="str">
         <f t="array" ref="G22">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="H22" s="46" t="str">
+      <c r="H22" s="40" t="str">
         <f t="array" ref="H22">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="I22" s="48" t="str">
+      <c r="I22" s="42" t="str">
         <f t="array" ref="I22">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
-      <c r="J22" s="49" t="str">
+      <c r="J22" s="43" t="str">
         <f t="array" ref="J22">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(17:17))),"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="str">
+      <c r="B23" s="38" t="str">
         <f t="array" ref="B23">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="C23" s="45" t="str">
+      <c r="C23" s="39" t="str">
         <f t="array" ref="C23">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="D23" s="46" t="str">
+      <c r="D23" s="40" t="str">
         <f t="array" ref="D23">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="E23" s="46" t="str">
+      <c r="E23" s="40" t="str">
         <f t="array" ref="E23">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="F23" s="47" t="str">
+      <c r="F23" s="41" t="str">
         <f t="array" ref="F23">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="G23" s="46" t="str">
+      <c r="G23" s="40" t="str">
         <f t="array" ref="G23">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="H23" s="46" t="str">
+      <c r="H23" s="40" t="str">
         <f t="array" ref="H23">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="I23" s="48" t="str">
+      <c r="I23" s="42" t="str">
         <f t="array" ref="I23">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
-      <c r="J23" s="49" t="str">
+      <c r="J23" s="43" t="str">
         <f t="array" ref="J23">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(18:18))),"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="str">
+      <c r="B24" s="38" t="str">
         <f t="array" ref="B24">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="C24" s="45" t="str">
+      <c r="C24" s="39" t="str">
         <f t="array" ref="C24">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="D24" s="46" t="str">
+      <c r="D24" s="40" t="str">
         <f t="array" ref="D24">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="E24" s="46" t="str">
+      <c r="E24" s="40" t="str">
         <f t="array" ref="E24">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="F24" s="47" t="str">
+      <c r="F24" s="41" t="str">
         <f t="array" ref="F24">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="G24" s="46" t="str">
+      <c r="G24" s="40" t="str">
         <f t="array" ref="G24">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="H24" s="46" t="str">
+      <c r="H24" s="40" t="str">
         <f t="array" ref="H24">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="I24" s="48" t="str">
+      <c r="I24" s="42" t="str">
         <f t="array" ref="I24">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
-      <c r="J24" s="49" t="str">
+      <c r="J24" s="43" t="str">
         <f t="array" ref="J24">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(19:19))),"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="str">
+      <c r="B25" s="38" t="str">
         <f t="array" ref="B25">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="C25" s="45" t="str">
+      <c r="C25" s="39" t="str">
         <f t="array" ref="C25">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="D25" s="46" t="str">
+      <c r="D25" s="40" t="str">
         <f t="array" ref="D25">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="E25" s="46" t="str">
+      <c r="E25" s="40" t="str">
         <f t="array" ref="E25">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="F25" s="47" t="str">
+      <c r="F25" s="41" t="str">
         <f t="array" ref="F25">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="G25" s="46" t="str">
+      <c r="G25" s="40" t="str">
         <f t="array" ref="G25">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="H25" s="46" t="str">
+      <c r="H25" s="40" t="str">
         <f t="array" ref="H25">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="I25" s="48" t="str">
+      <c r="I25" s="42" t="str">
         <f t="array" ref="I25">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
-      <c r="J25" s="49" t="str">
+      <c r="J25" s="43" t="str">
         <f t="array" ref="J25">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(20:20))),"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="str">
+      <c r="B26" s="38" t="str">
         <f t="array" ref="B26">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="C26" s="45" t="str">
+      <c r="C26" s="39" t="str">
         <f t="array" ref="C26">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="D26" s="46" t="str">
+      <c r="D26" s="40" t="str">
         <f t="array" ref="D26">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="E26" s="46" t="str">
+      <c r="E26" s="40" t="str">
         <f t="array" ref="E26">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="F26" s="47" t="str">
+      <c r="F26" s="41" t="str">
         <f t="array" ref="F26">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="G26" s="46" t="str">
+      <c r="G26" s="40" t="str">
         <f t="array" ref="G26">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="H26" s="46" t="str">
+      <c r="H26" s="40" t="str">
         <f t="array" ref="H26">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="I26" s="48" t="str">
+      <c r="I26" s="42" t="str">
         <f t="array" ref="I26">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
-      <c r="J26" s="49" t="str">
+      <c r="J26" s="43" t="str">
         <f t="array" ref="J26">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(21:21))),"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="44" t="str">
+      <c r="B27" s="38" t="str">
         <f t="array" ref="B27">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="C27" s="45" t="str">
+      <c r="C27" s="39" t="str">
         <f t="array" ref="C27">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="D27" s="46" t="str">
+      <c r="D27" s="40" t="str">
         <f t="array" ref="D27">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="E27" s="46" t="str">
+      <c r="E27" s="40" t="str">
         <f t="array" ref="E27">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="F27" s="47" t="str">
+      <c r="F27" s="41" t="str">
         <f t="array" ref="F27">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="G27" s="46" t="str">
+      <c r="G27" s="40" t="str">
         <f t="array" ref="G27">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="H27" s="46" t="str">
+      <c r="H27" s="40" t="str">
         <f t="array" ref="H27">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="I27" s="48" t="str">
+      <c r="I27" s="42" t="str">
         <f t="array" ref="I27">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
-      <c r="J27" s="49" t="str">
+      <c r="J27" s="43" t="str">
         <f t="array" ref="J27">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(22:22))),"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="str">
+      <c r="B28" s="38" t="str">
         <f t="array" ref="B28">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="C28" s="45" t="str">
+      <c r="C28" s="39" t="str">
         <f t="array" ref="C28">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="D28" s="46" t="str">
+      <c r="D28" s="40" t="str">
         <f t="array" ref="D28">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="E28" s="46" t="str">
+      <c r="E28" s="40" t="str">
         <f t="array" ref="E28">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="F28" s="47" t="str">
+      <c r="F28" s="41" t="str">
         <f t="array" ref="F28">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="G28" s="46" t="str">
+      <c r="G28" s="40" t="str">
         <f t="array" ref="G28">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="H28" s="46" t="str">
+      <c r="H28" s="40" t="str">
         <f t="array" ref="H28">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="I28" s="48" t="str">
+      <c r="I28" s="42" t="str">
         <f t="array" ref="I28">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
-      <c r="J28" s="49" t="str">
+      <c r="J28" s="43" t="str">
         <f t="array" ref="J28">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(23:23))),"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="str">
+      <c r="B29" s="38" t="str">
         <f t="array" ref="B29">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="C29" s="45" t="str">
+      <c r="C29" s="39" t="str">
         <f t="array" ref="C29">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="D29" s="46" t="str">
+      <c r="D29" s="40" t="str">
         <f t="array" ref="D29">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="E29" s="46" t="str">
+      <c r="E29" s="40" t="str">
         <f t="array" ref="E29">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="F29" s="47" t="str">
+      <c r="F29" s="41" t="str">
         <f t="array" ref="F29">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="G29" s="46" t="str">
+      <c r="G29" s="40" t="str">
         <f t="array" ref="G29">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="H29" s="46" t="str">
+      <c r="H29" s="40" t="str">
         <f t="array" ref="H29">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="I29" s="48" t="str">
+      <c r="I29" s="42" t="str">
         <f t="array" ref="I29">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
-      <c r="J29" s="49" t="str">
+      <c r="J29" s="43" t="str">
         <f t="array" ref="J29">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(24:24))),"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="str">
+      <c r="B30" s="38" t="str">
         <f t="array" ref="B30">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="C30" s="45" t="str">
+      <c r="C30" s="39" t="str">
         <f t="array" ref="C30">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="D30" s="46" t="str">
+      <c r="D30" s="40" t="str">
         <f t="array" ref="D30">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="E30" s="46" t="str">
+      <c r="E30" s="40" t="str">
         <f t="array" ref="E30">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="F30" s="47" t="str">
+      <c r="F30" s="41" t="str">
         <f t="array" ref="F30">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="G30" s="46" t="str">
+      <c r="G30" s="40" t="str">
         <f t="array" ref="G30">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="H30" s="46" t="str">
+      <c r="H30" s="40" t="str">
         <f t="array" ref="H30">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="I30" s="48" t="str">
+      <c r="I30" s="42" t="str">
         <f t="array" ref="I30">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
-      <c r="J30" s="49" t="str">
+      <c r="J30" s="43" t="str">
         <f t="array" ref="J30">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(25:25))),"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="str">
+      <c r="B31" s="38" t="str">
         <f t="array" ref="B31">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="C31" s="45" t="str">
+      <c r="C31" s="39" t="str">
         <f t="array" ref="C31">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="D31" s="46" t="str">
+      <c r="D31" s="40" t="str">
         <f t="array" ref="D31">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="E31" s="46" t="str">
+      <c r="E31" s="40" t="str">
         <f t="array" ref="E31">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="F31" s="47" t="str">
+      <c r="F31" s="41" t="str">
         <f t="array" ref="F31">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="G31" s="46" t="str">
+      <c r="G31" s="40" t="str">
         <f t="array" ref="G31">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="H31" s="46" t="str">
+      <c r="H31" s="40" t="str">
         <f t="array" ref="H31">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="I31" s="48" t="str">
+      <c r="I31" s="42" t="str">
         <f t="array" ref="I31">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
-      <c r="J31" s="49" t="str">
+      <c r="J31" s="43" t="str">
         <f t="array" ref="J31">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(26:26))),"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="str">
+      <c r="B32" s="38" t="str">
         <f t="array" ref="B32">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="C32" s="45" t="str">
+      <c r="C32" s="39" t="str">
         <f t="array" ref="C32">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="D32" s="46" t="str">
+      <c r="D32" s="40" t="str">
         <f t="array" ref="D32">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="E32" s="46" t="str">
+      <c r="E32" s="40" t="str">
         <f t="array" ref="E32">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="F32" s="47" t="str">
+      <c r="F32" s="41" t="str">
         <f t="array" ref="F32">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="G32" s="46" t="str">
+      <c r="G32" s="40" t="str">
         <f t="array" ref="G32">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="H32" s="46" t="str">
+      <c r="H32" s="40" t="str">
         <f t="array" ref="H32">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="I32" s="48" t="str">
+      <c r="I32" s="42" t="str">
         <f t="array" ref="I32">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
-      <c r="J32" s="49" t="str">
+      <c r="J32" s="43" t="str">
         <f t="array" ref="J32">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(27:27))),"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="44" t="str">
+      <c r="B33" s="38" t="str">
         <f t="array" ref="B33">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="C33" s="45" t="str">
+      <c r="C33" s="39" t="str">
         <f t="array" ref="C33">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="D33" s="46" t="str">
+      <c r="D33" s="40" t="str">
         <f t="array" ref="D33">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="E33" s="46" t="str">
+      <c r="E33" s="40" t="str">
         <f t="array" ref="E33">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="F33" s="47" t="str">
+      <c r="F33" s="41" t="str">
         <f t="array" ref="F33">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="G33" s="46" t="str">
+      <c r="G33" s="40" t="str">
         <f t="array" ref="G33">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="H33" s="46" t="str">
+      <c r="H33" s="40" t="str">
         <f t="array" ref="H33">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="I33" s="48" t="str">
+      <c r="I33" s="42" t="str">
         <f t="array" ref="I33">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
-      <c r="J33" s="49" t="str">
+      <c r="J33" s="43" t="str">
         <f t="array" ref="J33">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(28:28))),"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="44" t="str">
+      <c r="B34" s="38" t="str">
         <f t="array" ref="B34">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="C34" s="45" t="str">
+      <c r="C34" s="39" t="str">
         <f t="array" ref="C34">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="D34" s="46" t="str">
+      <c r="D34" s="40" t="str">
         <f t="array" ref="D34">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="E34" s="46" t="str">
+      <c r="E34" s="40" t="str">
         <f t="array" ref="E34">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="F34" s="47" t="str">
+      <c r="F34" s="41" t="str">
         <f t="array" ref="F34">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="G34" s="46" t="str">
+      <c r="G34" s="40" t="str">
         <f t="array" ref="G34">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="H34" s="46" t="str">
+      <c r="H34" s="40" t="str">
         <f t="array" ref="H34">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="I34" s="48" t="str">
+      <c r="I34" s="42" t="str">
         <f t="array" ref="I34">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
-      <c r="J34" s="49" t="str">
+      <c r="J34" s="43" t="str">
         <f t="array" ref="J34">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(29:29))),"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="44" t="str">
+      <c r="B35" s="38" t="str">
         <f t="array" ref="B35">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="C35" s="45" t="str">
+      <c r="C35" s="39" t="str">
         <f t="array" ref="C35">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="D35" s="46" t="str">
+      <c r="D35" s="40" t="str">
         <f t="array" ref="D35">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="E35" s="46" t="str">
+      <c r="E35" s="40" t="str">
         <f t="array" ref="E35">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="F35" s="47" t="str">
+      <c r="F35" s="41" t="str">
         <f t="array" ref="F35">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="G35" s="46" t="str">
+      <c r="G35" s="40" t="str">
         <f t="array" ref="G35">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="H35" s="46" t="str">
+      <c r="H35" s="40" t="str">
         <f t="array" ref="H35">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="I35" s="48" t="str">
+      <c r="I35" s="42" t="str">
         <f t="array" ref="I35">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
-      <c r="J35" s="49" t="str">
+      <c r="J35" s="43" t="str">
         <f t="array" ref="J35">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(30:30))),"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="str">
+      <c r="B36" s="38" t="str">
         <f t="array" ref="B36">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="C36" s="45" t="str">
+      <c r="C36" s="39" t="str">
         <f t="array" ref="C36">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="D36" s="46" t="str">
+      <c r="D36" s="40" t="str">
         <f t="array" ref="D36">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="E36" s="46" t="str">
+      <c r="E36" s="40" t="str">
         <f t="array" ref="E36">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="F36" s="47" t="str">
+      <c r="F36" s="41" t="str">
         <f t="array" ref="F36">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="G36" s="46" t="str">
+      <c r="G36" s="40" t="str">
         <f t="array" ref="G36">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="H36" s="46" t="str">
+      <c r="H36" s="40" t="str">
         <f t="array" ref="H36">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="I36" s="48" t="str">
+      <c r="I36" s="42" t="str">
         <f t="array" ref="I36">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
-      <c r="J36" s="49" t="str">
+      <c r="J36" s="43" t="str">
         <f t="array" ref="J36">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(31:31))),"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="44" t="str">
+      <c r="B37" s="38" t="str">
         <f t="array" ref="B37">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="C37" s="45" t="str">
+      <c r="C37" s="39" t="str">
         <f t="array" ref="C37">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="D37" s="46" t="str">
+      <c r="D37" s="40" t="str">
         <f t="array" ref="D37">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="E37" s="46" t="str">
+      <c r="E37" s="40" t="str">
         <f t="array" ref="E37">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="F37" s="47" t="str">
+      <c r="F37" s="41" t="str">
         <f t="array" ref="F37">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="G37" s="46" t="str">
+      <c r="G37" s="40" t="str">
         <f t="array" ref="G37">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="H37" s="46" t="str">
+      <c r="H37" s="40" t="str">
         <f t="array" ref="H37">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="I37" s="48" t="str">
+      <c r="I37" s="42" t="str">
         <f t="array" ref="I37">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
-      <c r="J37" s="49" t="str">
+      <c r="J37" s="43" t="str">
         <f t="array" ref="J37">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(32:32))),"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="44" t="str">
+      <c r="B38" s="38" t="str">
         <f t="array" ref="B38">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="C38" s="45" t="str">
+      <c r="C38" s="39" t="str">
         <f t="array" ref="C38">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="D38" s="46" t="str">
+      <c r="D38" s="40" t="str">
         <f t="array" ref="D38">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="E38" s="46" t="str">
+      <c r="E38" s="40" t="str">
         <f t="array" ref="E38">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="F38" s="47" t="str">
+      <c r="F38" s="41" t="str">
         <f t="array" ref="F38">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="G38" s="46" t="str">
+      <c r="G38" s="40" t="str">
         <f t="array" ref="G38">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="H38" s="46" t="str">
+      <c r="H38" s="40" t="str">
         <f t="array" ref="H38">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="I38" s="48" t="str">
+      <c r="I38" s="42" t="str">
         <f t="array" ref="I38">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
-      <c r="J38" s="49" t="str">
+      <c r="J38" s="43" t="str">
         <f t="array" ref="J38">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(33:33))),"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="44" t="str">
+      <c r="B39" s="38" t="str">
         <f t="array" ref="B39">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="C39" s="45" t="str">
+      <c r="C39" s="39" t="str">
         <f t="array" ref="C39">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="D39" s="46" t="str">
+      <c r="D39" s="40" t="str">
         <f t="array" ref="D39">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="E39" s="46" t="str">
+      <c r="E39" s="40" t="str">
         <f t="array" ref="E39">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="F39" s="47" t="str">
+      <c r="F39" s="41" t="str">
         <f t="array" ref="F39">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="G39" s="46" t="str">
+      <c r="G39" s="40" t="str">
         <f t="array" ref="G39">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="H39" s="46" t="str">
+      <c r="H39" s="40" t="str">
         <f t="array" ref="H39">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="I39" s="48" t="str">
+      <c r="I39" s="42" t="str">
         <f t="array" ref="I39">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
-      <c r="J39" s="49" t="str">
+      <c r="J39" s="43" t="str">
         <f t="array" ref="J39">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(34:34))),"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="44" t="str">
+      <c r="B40" s="38" t="str">
         <f t="array" ref="B40">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="C40" s="45" t="str">
+      <c r="C40" s="39" t="str">
         <f t="array" ref="C40">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="D40" s="46" t="str">
+      <c r="D40" s="40" t="str">
         <f t="array" ref="D40">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="E40" s="46" t="str">
+      <c r="E40" s="40" t="str">
         <f t="array" ref="E40">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="F40" s="47" t="str">
+      <c r="F40" s="41" t="str">
         <f t="array" ref="F40">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="G40" s="46" t="str">
+      <c r="G40" s="40" t="str">
         <f t="array" ref="G40">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="H40" s="46" t="str">
+      <c r="H40" s="40" t="str">
         <f t="array" ref="H40">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="I40" s="48" t="str">
+      <c r="I40" s="42" t="str">
         <f t="array" ref="I40">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
-      <c r="J40" s="49" t="str">
+      <c r="J40" s="43" t="str">
         <f t="array" ref="J40">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(35:35))),"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="44" t="str">
+      <c r="B41" s="38" t="str">
         <f t="array" ref="B41">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="C41" s="45" t="str">
+      <c r="C41" s="39" t="str">
         <f t="array" ref="C41">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="D41" s="46" t="str">
+      <c r="D41" s="40" t="str">
         <f t="array" ref="D41">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="E41" s="46" t="str">
+      <c r="E41" s="40" t="str">
         <f t="array" ref="E41">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="F41" s="47" t="str">
+      <c r="F41" s="41" t="str">
         <f t="array" ref="F41">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="G41" s="46" t="str">
+      <c r="G41" s="40" t="str">
         <f t="array" ref="G41">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="H41" s="46" t="str">
+      <c r="H41" s="40" t="str">
         <f t="array" ref="H41">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="I41" s="48" t="str">
+      <c r="I41" s="42" t="str">
         <f t="array" ref="I41">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
-      <c r="J41" s="49" t="str">
+      <c r="J41" s="43" t="str">
         <f t="array" ref="J41">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(36:36))),"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="44" t="str">
+      <c r="B42" s="38" t="str">
         <f t="array" ref="B42">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="C42" s="45" t="str">
+      <c r="C42" s="39" t="str">
         <f t="array" ref="C42">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="D42" s="46" t="str">
+      <c r="D42" s="40" t="str">
         <f t="array" ref="D42">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="E42" s="46" t="str">
+      <c r="E42" s="40" t="str">
         <f t="array" ref="E42">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="F42" s="47" t="str">
+      <c r="F42" s="41" t="str">
         <f t="array" ref="F42">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="G42" s="46" t="str">
+      <c r="G42" s="40" t="str">
         <f t="array" ref="G42">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="H42" s="46" t="str">
+      <c r="H42" s="40" t="str">
         <f t="array" ref="H42">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="I42" s="48" t="str">
+      <c r="I42" s="42" t="str">
         <f t="array" ref="I42">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
-      <c r="J42" s="49" t="str">
+      <c r="J42" s="43" t="str">
         <f t="array" ref="J42">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(37:37))),"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="44" t="str">
+      <c r="B43" s="38" t="str">
         <f t="array" ref="B43">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="C43" s="45" t="str">
+      <c r="C43" s="39" t="str">
         <f t="array" ref="C43">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="D43" s="46" t="str">
+      <c r="D43" s="40" t="str">
         <f t="array" ref="D43">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="E43" s="46" t="str">
+      <c r="E43" s="40" t="str">
         <f t="array" ref="E43">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="F43" s="47" t="str">
+      <c r="F43" s="41" t="str">
         <f t="array" ref="F43">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="G43" s="46" t="str">
+      <c r="G43" s="40" t="str">
         <f t="array" ref="G43">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="H43" s="46" t="str">
+      <c r="H43" s="40" t="str">
         <f t="array" ref="H43">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="I43" s="48" t="str">
+      <c r="I43" s="42" t="str">
         <f t="array" ref="I43">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
-      <c r="J43" s="49" t="str">
+      <c r="J43" s="43" t="str">
         <f t="array" ref="J43">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(38:38))),"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="44" t="str">
+      <c r="B44" s="38" t="str">
         <f t="array" ref="B44">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="C44" s="45" t="str">
+      <c r="C44" s="39" t="str">
         <f t="array" ref="C44">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="D44" s="46" t="str">
+      <c r="D44" s="40" t="str">
         <f t="array" ref="D44">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="E44" s="46" t="str">
+      <c r="E44" s="40" t="str">
         <f t="array" ref="E44">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="F44" s="47" t="str">
+      <c r="F44" s="41" t="str">
         <f t="array" ref="F44">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="G44" s="46" t="str">
+      <c r="G44" s="40" t="str">
         <f t="array" ref="G44">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="H44" s="46" t="str">
+      <c r="H44" s="40" t="str">
         <f t="array" ref="H44">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="I44" s="48" t="str">
+      <c r="I44" s="42" t="str">
         <f t="array" ref="I44">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
-      <c r="J44" s="49" t="str">
+      <c r="J44" s="43" t="str">
         <f t="array" ref="J44">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(39:39))),"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="44" t="str">
+      <c r="B45" s="38" t="str">
         <f t="array" ref="B45">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="C45" s="45" t="str">
+      <c r="C45" s="39" t="str">
         <f t="array" ref="C45">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="D45" s="46" t="str">
+      <c r="D45" s="40" t="str">
         <f t="array" ref="D45">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="E45" s="46" t="str">
+      <c r="E45" s="40" t="str">
         <f t="array" ref="E45">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="F45" s="47" t="str">
+      <c r="F45" s="41" t="str">
         <f t="array" ref="F45">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="G45" s="46" t="str">
+      <c r="G45" s="40" t="str">
         <f t="array" ref="G45">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="H45" s="46" t="str">
+      <c r="H45" s="40" t="str">
         <f t="array" ref="H45">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="I45" s="48" t="str">
+      <c r="I45" s="42" t="str">
         <f t="array" ref="I45">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
-      <c r="J45" s="49" t="str">
+      <c r="J45" s="43" t="str">
         <f t="array" ref="J45">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(40:40))),"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="44" t="str">
+      <c r="B46" s="38" t="str">
         <f t="array" ref="B46">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="C46" s="45" t="str">
+      <c r="C46" s="39" t="str">
         <f t="array" ref="C46">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="D46" s="46" t="str">
+      <c r="D46" s="40" t="str">
         <f t="array" ref="D46">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="E46" s="46" t="str">
+      <c r="E46" s="40" t="str">
         <f t="array" ref="E46">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="F46" s="47" t="str">
+      <c r="F46" s="41" t="str">
         <f t="array" ref="F46">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="G46" s="46" t="str">
+      <c r="G46" s="40" t="str">
         <f t="array" ref="G46">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="H46" s="46" t="str">
+      <c r="H46" s="40" t="str">
         <f t="array" ref="H46">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="I46" s="48" t="str">
+      <c r="I46" s="42" t="str">
         <f t="array" ref="I46">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
-      <c r="J46" s="49" t="str">
+      <c r="J46" s="43" t="str">
         <f t="array" ref="J46">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(41:41))),"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="44" t="str">
+      <c r="B47" s="38" t="str">
         <f t="array" ref="B47">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="C47" s="45" t="str">
+      <c r="C47" s="39" t="str">
         <f t="array" ref="C47">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="D47" s="46" t="str">
+      <c r="D47" s="40" t="str">
         <f t="array" ref="D47">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="E47" s="46" t="str">
+      <c r="E47" s="40" t="str">
         <f t="array" ref="E47">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="F47" s="47" t="str">
+      <c r="F47" s="41" t="str">
         <f t="array" ref="F47">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="G47" s="46" t="str">
+      <c r="G47" s="40" t="str">
         <f t="array" ref="G47">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="H47" s="46" t="str">
+      <c r="H47" s="40" t="str">
         <f t="array" ref="H47">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="I47" s="48" t="str">
+      <c r="I47" s="42" t="str">
         <f t="array" ref="I47">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
-      <c r="J47" s="49" t="str">
+      <c r="J47" s="43" t="str">
         <f t="array" ref="J47">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(42:42))),"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="44" t="str">
+      <c r="B48" s="38" t="str">
         <f t="array" ref="B48">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="C48" s="45" t="str">
+      <c r="C48" s="39" t="str">
         <f t="array" ref="C48">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="D48" s="46" t="str">
+      <c r="D48" s="40" t="str">
         <f t="array" ref="D48">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="E48" s="46" t="str">
+      <c r="E48" s="40" t="str">
         <f t="array" ref="E48">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="F48" s="47" t="str">
+      <c r="F48" s="41" t="str">
         <f t="array" ref="F48">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="G48" s="46" t="str">
+      <c r="G48" s="40" t="str">
         <f t="array" ref="G48">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="H48" s="46" t="str">
+      <c r="H48" s="40" t="str">
         <f t="array" ref="H48">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="I48" s="48" t="str">
+      <c r="I48" s="42" t="str">
         <f t="array" ref="I48">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
-      <c r="J48" s="49" t="str">
+      <c r="J48" s="43" t="str">
         <f t="array" ref="J48">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(43:43))),"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="44" t="str">
+      <c r="B49" s="38" t="str">
         <f t="array" ref="B49">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="C49" s="45" t="str">
+      <c r="C49" s="39" t="str">
         <f t="array" ref="C49">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="D49" s="46" t="str">
+      <c r="D49" s="40" t="str">
         <f t="array" ref="D49">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="E49" s="46" t="str">
+      <c r="E49" s="40" t="str">
         <f t="array" ref="E49">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="F49" s="47" t="str">
+      <c r="F49" s="41" t="str">
         <f t="array" ref="F49">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="G49" s="46" t="str">
+      <c r="G49" s="40" t="str">
         <f t="array" ref="G49">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="H49" s="46" t="str">
+      <c r="H49" s="40" t="str">
         <f t="array" ref="H49">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="I49" s="48" t="str">
+      <c r="I49" s="42" t="str">
         <f t="array" ref="I49">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
-      <c r="J49" s="49" t="str">
+      <c r="J49" s="43" t="str">
         <f t="array" ref="J49">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(44:44))),"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="44" t="str">
+      <c r="B50" s="38" t="str">
         <f t="array" ref="B50">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="C50" s="45" t="str">
+      <c r="C50" s="39" t="str">
         <f t="array" ref="C50">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="D50" s="46" t="str">
+      <c r="D50" s="40" t="str">
         <f t="array" ref="D50">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="E50" s="46" t="str">
+      <c r="E50" s="40" t="str">
         <f t="array" ref="E50">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="F50" s="47" t="str">
+      <c r="F50" s="41" t="str">
         <f t="array" ref="F50">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="G50" s="46" t="str">
+      <c r="G50" s="40" t="str">
         <f t="array" ref="G50">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="H50" s="46" t="str">
+      <c r="H50" s="40" t="str">
         <f t="array" ref="H50">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="I50" s="48" t="str">
+      <c r="I50" s="42" t="str">
         <f t="array" ref="I50">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
-      <c r="J50" s="49" t="str">
+      <c r="J50" s="43" t="str">
         <f t="array" ref="J50">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(45:45))),"")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="44" t="str">
+      <c r="B51" s="38" t="str">
         <f t="array" ref="B51">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="C51" s="45" t="str">
+      <c r="C51" s="39" t="str">
         <f t="array" ref="C51">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="D51" s="46" t="str">
+      <c r="D51" s="40" t="str">
         <f t="array" ref="D51">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="E51" s="46" t="str">
+      <c r="E51" s="40" t="str">
         <f t="array" ref="E51">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="F51" s="47" t="str">
+      <c r="F51" s="41" t="str">
         <f t="array" ref="F51">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="G51" s="46" t="str">
+      <c r="G51" s="40" t="str">
         <f t="array" ref="G51">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="H51" s="46" t="str">
+      <c r="H51" s="40" t="str">
         <f t="array" ref="H51">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="I51" s="48" t="str">
+      <c r="I51" s="42" t="str">
         <f t="array" ref="I51">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
-      <c r="J51" s="49" t="str">
+      <c r="J51" s="43" t="str">
         <f t="array" ref="J51">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(46:46))),"")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="str">
+      <c r="B52" s="38" t="str">
         <f t="array" ref="B52">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="C52" s="45" t="str">
+      <c r="C52" s="39" t="str">
         <f t="array" ref="C52">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="D52" s="46" t="str">
+      <c r="D52" s="40" t="str">
         <f t="array" ref="D52">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="E52" s="46" t="str">
+      <c r="E52" s="40" t="str">
         <f t="array" ref="E52">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="F52" s="47" t="str">
+      <c r="F52" s="41" t="str">
         <f t="array" ref="F52">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="G52" s="46" t="str">
+      <c r="G52" s="40" t="str">
         <f t="array" ref="G52">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="H52" s="46" t="str">
+      <c r="H52" s="40" t="str">
         <f t="array" ref="H52">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="I52" s="48" t="str">
+      <c r="I52" s="42" t="str">
         <f t="array" ref="I52">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
-      <c r="J52" s="49" t="str">
+      <c r="J52" s="43" t="str">
         <f t="array" ref="J52">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(47:47))),"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="44" t="str">
+      <c r="B53" s="38" t="str">
         <f t="array" ref="B53">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="C53" s="45" t="str">
+      <c r="C53" s="39" t="str">
         <f t="array" ref="C53">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="D53" s="46" t="str">
+      <c r="D53" s="40" t="str">
         <f t="array" ref="D53">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="E53" s="46" t="str">
+      <c r="E53" s="40" t="str">
         <f t="array" ref="E53">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="F53" s="47" t="str">
+      <c r="F53" s="41" t="str">
         <f t="array" ref="F53">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="G53" s="46" t="str">
+      <c r="G53" s="40" t="str">
         <f t="array" ref="G53">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="H53" s="46" t="str">
+      <c r="H53" s="40" t="str">
         <f t="array" ref="H53">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="I53" s="48" t="str">
+      <c r="I53" s="42" t="str">
         <f t="array" ref="I53">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
-      <c r="J53" s="49" t="str">
+      <c r="J53" s="43" t="str">
         <f t="array" ref="J53">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(48:48))),"")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="44" t="str">
+      <c r="B54" s="38" t="str">
         <f t="array" ref="B54">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="C54" s="45" t="str">
+      <c r="C54" s="39" t="str">
         <f t="array" ref="C54">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="D54" s="46" t="str">
+      <c r="D54" s="40" t="str">
         <f t="array" ref="D54">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="E54" s="46" t="str">
+      <c r="E54" s="40" t="str">
         <f t="array" ref="E54">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="F54" s="47" t="str">
+      <c r="F54" s="41" t="str">
         <f t="array" ref="F54">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="G54" s="46" t="str">
+      <c r="G54" s="40" t="str">
         <f t="array" ref="G54">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="H54" s="46" t="str">
+      <c r="H54" s="40" t="str">
         <f t="array" ref="H54">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="I54" s="48" t="str">
+      <c r="I54" s="42" t="str">
         <f t="array" ref="I54">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
-      <c r="J54" s="49" t="str">
+      <c r="J54" s="43" t="str">
         <f t="array" ref="J54">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(49:49))),"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="50" t="str">
+      <c r="B55" s="44" t="str">
         <f t="array" ref="B55">IFERROR(INDEX(R_TABELA[DESCRIÇÃO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DESCRIÇÃO])-ROW(INDEX(R_TABELA[DESCRIÇÃO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="C55" s="51" t="str">
+      <c r="C55" s="45" t="str">
         <f t="array" ref="C55">IFERROR(INDEX(R_TABELA[VALOR],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[VALOR])-ROW(INDEX(R_TABELA[VALOR],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="D55" s="52" t="str">
+      <c r="D55" s="46" t="str">
         <f t="array" ref="D55">IFERROR(INDEX(R_TABELA[STATUS],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[STATUS])-ROW(INDEX(R_TABELA[STATUS],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="E55" s="52" t="str">
+      <c r="E55" s="46" t="str">
         <f t="array" ref="E55">IFERROR(INDEX(R_TABELA[CATEGORIA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[CATEGORIA])-ROW(INDEX(R_TABELA[CATEGORIA],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="F55" s="53" t="str">
+      <c r="F55" s="47" t="str">
         <f t="array" ref="F55">IFERROR(INDEX(R_TABELA[DATA DE VENCIMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[DATA DE VENCIMENTO])-ROW(INDEX(R_TABELA[DATA DE VENCIMENTO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="G55" s="52" t="str">
+      <c r="G55" s="46" t="str">
         <f t="array" ref="G55">IFERROR(INDEX(R_TABELA[FORMA DE PAGAMENTO],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[FORMA DE PAGAMENTO])-ROW(INDEX(R_TABELA[FORMA DE PAGAMENTO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="H55" s="52" t="str">
+      <c r="H55" s="46" t="str">
         <f t="array" ref="H55">IFERROR(INDEX(R_TABELA[PARCELA],SMALL(IF((MONTH(R_TABELA[DATA DE VENCIMENTO])=$C$2)*(YEAR(R_TABELA[DATA DE VENCIMENTO])=$C$3),ROW(R_TABELA[PARCELA])-ROW(INDEX(R_TABELA[PARCELA],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="I55" s="54" t="str">
+      <c r="I55" s="48" t="str">
         <f t="array" ref="I55">IFERROR(INDEX(R_ENTRADA[DESCRIÇÃO],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[DESCRIÇÃO])-ROW(INDEX(R_ENTRADA[DESCRIÇÃO],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
-      <c r="J55" s="55" t="str">
+      <c r="J55" s="49" t="str">
         <f t="array" ref="J55">IFERROR(INDEX(R_ENTRADA[VALOR],SMALL(IF((R_ENTRADA[MÊS]=$C$2)*(R_ENTRADA[ANO]=$C$3),ROW(R_ENTRADA[VALOR])-ROW(INDEX(R_ENTRADA[VALOR],1,1))+1),ROW(50:50))),"")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="LQp5WlmghsKrXuUQuTezrr0BVasqZzAh4HUmkEA5GEKdKi5ok90wkVU4a+lQ/P9vDKf0On6QWWHy1QVBpkZVFw==" saltValue="Rj2PXw5mWec3MMiY11yfeg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="D4:G4"/>
@@ -5124,13 +5069,13 @@
     <mergeCell ref="M16:M17"/>
   </mergeCells>
   <conditionalFormatting sqref="M16:M17">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="lessThanOrEqual">
       <formula>$H$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>$H$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5681,49 +5626,33 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="C1 C17:C161">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+  <conditionalFormatting sqref="C1:C161">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C161">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+  <conditionalFormatting sqref="C2:C161">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C162:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"INVESTIMENTO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>"PARCELADO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>"PENDENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
-      <formula>"PAGO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"INVESTIMENTO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"PARCELADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"PENDENTE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Atualização recente da planilha financeira
</commit_message>
<xml_diff>
--- a/planilha_financeira.xlsx
+++ b/planilha_financeira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jean\Desktop\planilha_financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E9963-C67B-47FA-991C-4E5205A028C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51C052E-61D8-49BA-B8A8-7A6AF5E59235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37E1AD45-33B4-4EA6-A144-DD0226F01E22}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSULTA" sheetId="20" r:id="rId1"/>
@@ -3030,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D74486-E613-4DD7-8E3C-257D31A44268}">
   <dimension ref="B1:M56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,7 +5088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262A3E2A-86CA-4231-B82B-405B67DE33BC}">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>

</xml_diff>